<commit_message>
add new LAOs biorefinery, add tests for sugarcane, and readmes to all biorefineries
</commit_message>
<xml_diff>
--- a/BioSTEAM 2.x.x/biorefineries/cornstover/_humbird2011.xlsx
+++ b/BioSTEAM 2.x.x/biorefineries/cornstover/_humbird2011.xlsx
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="156" uniqueCount="51">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="153" uniqueCount="50">
   <si>
     <t>CEPCI</t>
   </si>
@@ -179,9 +179,6 @@
   </si>
   <si>
     <t>Ammonia addition tank</t>
-  </si>
-  <si>
-    <t>Baghouse bags</t>
   </si>
   <si>
     <t>Bag unloader</t>
@@ -249,7 +246,7 @@
     <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="32">
+  <cellXfs count="30">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -324,12 +321,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
@@ -658,7 +649,7 @@
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="62" zoomScaleNormal="62" workbookViewId="0">
       <pane xSplit="1" topLeftCell="AD1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="AL14" sqref="AL14"/>
+      <selection pane="topRight" activeCell="AM9" sqref="AM9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -696,10 +687,10 @@
       <c r="B1" s="6" t="s">
         <v>27</v>
       </c>
-      <c r="C1" s="30" t="s">
+      <c r="C1" s="28" t="s">
         <v>33</v>
       </c>
-      <c r="D1" s="30"/>
+      <c r="D1" s="28"/>
       <c r="E1" s="6" t="s">
         <v>19</v>
       </c>
@@ -709,27 +700,27 @@
       <c r="G1" s="6" t="s">
         <v>34</v>
       </c>
-      <c r="H1" s="30" t="s">
+      <c r="H1" s="28" t="s">
         <v>45</v>
       </c>
-      <c r="I1" s="30"/>
-      <c r="J1" s="30"/>
-      <c r="K1" s="30" t="s">
+      <c r="I1" s="28"/>
+      <c r="J1" s="28"/>
+      <c r="K1" s="28" t="s">
         <v>35</v>
       </c>
-      <c r="L1" s="30"/>
-      <c r="M1" s="30"/>
-      <c r="N1" s="30" t="s">
+      <c r="L1" s="28"/>
+      <c r="M1" s="28"/>
+      <c r="N1" s="28" t="s">
         <v>48</v>
       </c>
-      <c r="O1" s="30"/>
+      <c r="O1" s="28"/>
       <c r="P1" s="5" t="s">
         <v>47</v>
       </c>
-      <c r="Q1" s="30" t="s">
+      <c r="Q1" s="28" t="s">
         <v>36</v>
       </c>
-      <c r="R1" s="30"/>
+      <c r="R1" s="28"/>
       <c r="S1" s="6" t="s">
         <v>37</v>
       </c>
@@ -745,38 +736,37 @@
       <c r="W1" s="4" t="s">
         <v>40</v>
       </c>
-      <c r="X1" s="31" t="s">
+      <c r="X1" s="29" t="s">
         <v>41</v>
       </c>
-      <c r="Y1" s="31"/>
-      <c r="Z1" s="31"/>
+      <c r="Y1" s="29"/>
+      <c r="Z1" s="29"/>
       <c r="AA1" s="15" t="s">
         <v>42</v>
       </c>
       <c r="AB1" s="15" t="s">
         <v>43</v>
       </c>
-      <c r="AC1" s="31" t="s">
+      <c r="AC1" s="29" t="s">
         <v>44</v>
       </c>
-      <c r="AD1" s="31"/>
-      <c r="AE1" s="31"/>
-      <c r="AF1" s="30" t="s">
+      <c r="AD1" s="29"/>
+      <c r="AE1" s="29"/>
+      <c r="AF1" s="28" t="s">
         <v>29</v>
       </c>
-      <c r="AG1" s="30"/>
-      <c r="AH1" s="30"/>
-      <c r="AI1" s="30" t="s">
+      <c r="AG1" s="28"/>
+      <c r="AH1" s="28"/>
+      <c r="AI1" s="28" t="s">
         <v>30</v>
       </c>
-      <c r="AJ1" s="30"/>
-      <c r="AK1" s="30"/>
-      <c r="AL1" s="30"/>
-      <c r="AM1" s="30"/>
-      <c r="AN1" s="30" t="s">
+      <c r="AJ1" s="28"/>
+      <c r="AK1" s="28"/>
+      <c r="AL1" s="28"/>
+      <c r="AM1" s="28" t="s">
         <v>31</v>
       </c>
-      <c r="AO1" s="30"/>
+      <c r="AN1" s="28"/>
       <c r="AP1" s="26"/>
     </row>
     <row r="2" spans="1:42" s="7" customFormat="1" x14ac:dyDescent="0.3">
@@ -891,16 +881,13 @@
       <c r="AK2" s="23" t="s">
         <v>15</v>
       </c>
-      <c r="AL2" s="28" t="s">
+      <c r="AL2" s="7" t="s">
         <v>49</v>
       </c>
-      <c r="AM2" s="7" t="s">
-        <v>50</v>
+      <c r="AM2" s="24" t="s">
+        <v>8</v>
       </c>
       <c r="AN2" s="24" t="s">
-        <v>8</v>
-      </c>
-      <c r="AO2" s="24" t="s">
         <v>16</v>
       </c>
     </row>
@@ -1016,16 +1003,13 @@
       <c r="AK3" s="23" t="s">
         <v>6</v>
       </c>
-      <c r="AL3" s="28" t="s">
-        <v>6</v>
-      </c>
-      <c r="AM3" s="23" t="s">
+      <c r="AL3" s="23" t="s">
+        <v>6</v>
+      </c>
+      <c r="AM3" s="24" t="s">
         <v>6</v>
       </c>
       <c r="AN3" s="24" t="s">
-        <v>6</v>
-      </c>
-      <c r="AO3" s="24" t="s">
         <v>6</v>
       </c>
     </row>
@@ -1141,16 +1125,13 @@
       <c r="AK4" s="22" t="s">
         <v>7</v>
       </c>
-      <c r="AL4" s="29" t="s">
-        <v>7</v>
-      </c>
-      <c r="AM4" s="22" t="s">
+      <c r="AL4" s="22" t="s">
+        <v>7</v>
+      </c>
+      <c r="AM4" s="25" t="s">
         <v>7</v>
       </c>
       <c r="AN4" s="25" t="s">
-        <v>7</v>
-      </c>
-      <c r="AO4" s="25" t="s">
         <v>7</v>
       </c>
     </row>
@@ -1266,16 +1247,13 @@
       <c r="AK5" s="23">
         <v>163</v>
       </c>
-      <c r="AL5" s="28">
+      <c r="AL5" s="23">
         <v>163</v>
       </c>
-      <c r="AM5" s="23">
-        <v>163</v>
+      <c r="AM5" s="24">
+        <v>8343</v>
       </c>
       <c r="AN5" s="24">
-        <v>8343</v>
-      </c>
-      <c r="AO5" s="24">
         <v>8343</v>
       </c>
     </row>
@@ -1406,16 +1384,13 @@
       <c r="AK6" s="23" t="b">
         <v>0</v>
       </c>
-      <c r="AL6" s="28" t="b">
-        <v>0</v>
-      </c>
-      <c r="AM6" s="23" t="b">
+      <c r="AL6" s="23" t="b">
+        <v>0</v>
+      </c>
+      <c r="AM6" s="24" t="b">
         <v>0</v>
       </c>
       <c r="AN6" s="24" t="b">
-        <v>0</v>
-      </c>
-      <c r="AO6" s="24" t="b">
         <v>0</v>
       </c>
     </row>
@@ -1531,16 +1506,13 @@
       <c r="AK7" s="23">
         <v>522</v>
       </c>
-      <c r="AL7" s="28">
-        <v>522</v>
-      </c>
-      <c r="AM7" s="23">
+      <c r="AL7" s="23">
+        <v>522</v>
+      </c>
+      <c r="AM7" s="24">
         <v>522</v>
       </c>
       <c r="AN7" s="24">
-        <v>522</v>
-      </c>
-      <c r="AO7" s="24">
         <v>522</v>
       </c>
     </row>
@@ -1657,15 +1629,12 @@
         <v>9800</v>
       </c>
       <c r="AL8" s="8">
-        <v>466183</v>
+        <v>30000</v>
       </c>
       <c r="AM8" s="8">
-        <v>30000</v>
+        <v>803000</v>
       </c>
       <c r="AN8" s="8">
-        <v>803000</v>
-      </c>
-      <c r="AO8" s="8">
         <v>15000</v>
       </c>
     </row>
@@ -1781,16 +1750,13 @@
       <c r="AK9" s="23">
         <v>0.5</v>
       </c>
-      <c r="AL9" s="28">
-        <v>1</v>
-      </c>
-      <c r="AM9" s="23">
+      <c r="AL9" s="23">
         <v>0.6</v>
       </c>
+      <c r="AM9" s="24">
+        <v>0.7</v>
+      </c>
       <c r="AN9" s="24">
-        <v>0.7</v>
-      </c>
-      <c r="AO9" s="24">
         <v>0.8</v>
       </c>
     </row>
@@ -1926,9 +1892,6 @@
         <v>0</v>
       </c>
       <c r="AN10" s="10">
-        <v>0</v>
-      </c>
-      <c r="AO10" s="10">
         <f>125*0.7547</f>
         <v>94.337500000000006</v>
       </c>
@@ -2045,16 +2008,13 @@
       <c r="AK11" s="23">
         <v>1.5</v>
       </c>
-      <c r="AL11" s="28">
-        <v>1</v>
-      </c>
-      <c r="AM11" s="23">
+      <c r="AL11" s="23">
         <v>1.7</v>
       </c>
+      <c r="AM11" s="24">
+        <v>1.8</v>
+      </c>
       <c r="AN11" s="24">
-        <v>1.8</v>
-      </c>
-      <c r="AO11" s="24">
         <v>1.7</v>
       </c>
     </row>
@@ -2170,16 +2130,13 @@
       <c r="AK12" s="27" t="b">
         <v>0</v>
       </c>
-      <c r="AL12" s="28" t="b">
+      <c r="AL12" s="27" t="b">
         <v>0</v>
       </c>
       <c r="AM12" s="27" t="b">
         <v>0</v>
       </c>
       <c r="AN12" s="27" t="b">
-        <v>0</v>
-      </c>
-      <c r="AO12" s="27" t="b">
         <v>0</v>
       </c>
     </row>
@@ -2203,6 +2160,8 @@
     </row>
   </sheetData>
   <mergeCells count="10">
+    <mergeCell ref="AI1:AL1"/>
+    <mergeCell ref="AM1:AN1"/>
     <mergeCell ref="C1:D1"/>
     <mergeCell ref="N1:O1"/>
     <mergeCell ref="H1:J1"/>
@@ -2211,8 +2170,6 @@
     <mergeCell ref="AC1:AE1"/>
     <mergeCell ref="X1:Z1"/>
     <mergeCell ref="K1:M1"/>
-    <mergeCell ref="AN1:AO1"/>
-    <mergeCell ref="AI1:AM1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
bump up version and minor fixes to tests
</commit_message>
<xml_diff>
--- a/BioSTEAM 2.x.x/biorefineries/cornstover/_humbird2011.xlsx
+++ b/BioSTEAM 2.x.x/biorefineries/cornstover/_humbird2011.xlsx
@@ -1,22 +1,23 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="7" rupBuild="14420"/>
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23426"/>
+  <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\yrc2\OneDrive\Code\Bioindustrial-Park\BioSTEAM 2.x.x\biorefineries\cornstover\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/733a0933307f0df0/Code/Bioindustrial-Park/BioSTEAM 2.x.x/biorefineries/cornstover/"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="1" documentId="11_93738BBF658B224CE52DD40E9AAED54DBB468F57" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{A0296A15-CD74-4E0D-9116-30CAC8267C48}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="25824" windowHeight="14016"/>
+    <workbookView xWindow="2508" yWindow="1380" windowWidth="20532" windowHeight="10980" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId2"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -24,7 +25,10 @@
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
         <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -187,7 +191,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="3">
     <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
@@ -644,7 +648,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AP27"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="62" zoomScaleNormal="62" workbookViewId="0">
@@ -677,7 +681,7 @@
     <col min="37" max="37" width="11.77734375" customWidth="1"/>
     <col min="38" max="38" width="16.109375" bestFit="1" customWidth="1"/>
     <col min="39" max="39" width="14.109375" customWidth="1"/>
-    <col min="40" max="40" width="9.88671875" bestFit="1" customWidth="1"/>
+    <col min="40" max="40" width="10.5546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:42" s="3" customFormat="1" x14ac:dyDescent="0.3">
@@ -2177,7 +2181,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -2194,7 +2198,7 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:B3"/>
   <sheetViews>
     <sheetView workbookViewId="0">

</xml_diff>

<commit_message>
add new preprocessing units and reconfigure lactic and ethanol_adipic biorefineries
</commit_message>
<xml_diff>
--- a/BioSTEAM 2.x.x/biorefineries/cornstover/_humbird2011.xlsx
+++ b/BioSTEAM 2.x.x/biorefineries/cornstover/_humbird2011.xlsx
@@ -1,22 +1,23 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="7" rupBuild="14420"/>
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11213"/>
+  <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\yrc2\OneDrive\Code\Bioindustrial-Park\BioSTEAM 2.x.x\biorefineries\cornstover\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/bfca01abaf64aab7/Coding/bp/BioSTEAM 2.x.x/biorefineries/cornstover/"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="1" documentId="11_93738BBF658B224CE52DD40E9AAED54DBB468F57" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{57696482-969E-F749-AC74-931B1CDEEAC9}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="25824" windowHeight="14016"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="25820" windowHeight="14020" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId2"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -24,7 +25,10 @@
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
         <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -187,7 +191,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="3">
     <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
@@ -246,7 +250,7 @@
     <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="30">
+  <cellXfs count="29">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -319,7 +323,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -644,53 +647,53 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AP27"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:AN27"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="62" zoomScaleNormal="62" workbookViewId="0">
       <pane xSplit="1" topLeftCell="AD1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="AM9" sqref="AM9"/>
+      <selection pane="topRight" activeCell="AS11" sqref="AS11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="24.77734375" customWidth="1"/>
-    <col min="2" max="5" width="24.77734375" style="2" customWidth="1"/>
-    <col min="6" max="6" width="29.77734375" style="2" customWidth="1"/>
-    <col min="7" max="7" width="35.109375" style="2" customWidth="1"/>
-    <col min="8" max="18" width="24.77734375" style="2" customWidth="1"/>
+    <col min="1" max="1" width="24.83203125" customWidth="1"/>
+    <col min="2" max="5" width="24.83203125" style="2" customWidth="1"/>
+    <col min="6" max="6" width="29.83203125" style="2" customWidth="1"/>
+    <col min="7" max="7" width="35.1640625" style="2" customWidth="1"/>
+    <col min="8" max="18" width="24.83203125" style="2" customWidth="1"/>
     <col min="19" max="19" width="38.33203125" style="2" customWidth="1"/>
     <col min="20" max="20" width="36.33203125" customWidth="1"/>
-    <col min="21" max="21" width="24.77734375" customWidth="1"/>
+    <col min="21" max="21" width="24.83203125" customWidth="1"/>
     <col min="22" max="22" width="36.6640625" customWidth="1"/>
-    <col min="23" max="23" width="41.21875" customWidth="1"/>
-    <col min="24" max="26" width="24.77734375" customWidth="1"/>
-    <col min="27" max="27" width="29.44140625" customWidth="1"/>
-    <col min="28" max="28" width="32.109375" customWidth="1"/>
+    <col min="23" max="23" width="41.1640625" customWidth="1"/>
+    <col min="24" max="26" width="24.83203125" customWidth="1"/>
+    <col min="27" max="27" width="29.5" customWidth="1"/>
+    <col min="28" max="28" width="32.1640625" customWidth="1"/>
     <col min="29" max="29" width="24.6640625" bestFit="1" customWidth="1"/>
-    <col min="30" max="30" width="9.88671875" bestFit="1" customWidth="1"/>
-    <col min="31" max="31" width="10.21875" customWidth="1"/>
-    <col min="32" max="32" width="9.88671875" bestFit="1" customWidth="1"/>
-    <col min="34" max="34" width="9.88671875" bestFit="1" customWidth="1"/>
-    <col min="35" max="35" width="11.5546875" bestFit="1" customWidth="1"/>
-    <col min="36" max="36" width="10.88671875" bestFit="1" customWidth="1"/>
-    <col min="37" max="37" width="11.77734375" customWidth="1"/>
-    <col min="38" max="38" width="16.109375" bestFit="1" customWidth="1"/>
-    <col min="39" max="39" width="14.109375" customWidth="1"/>
-    <col min="40" max="40" width="9.88671875" bestFit="1" customWidth="1"/>
+    <col min="30" max="30" width="9.83203125" bestFit="1" customWidth="1"/>
+    <col min="31" max="31" width="10.1640625" customWidth="1"/>
+    <col min="32" max="32" width="9.83203125" bestFit="1" customWidth="1"/>
+    <col min="34" max="34" width="9.83203125" bestFit="1" customWidth="1"/>
+    <col min="35" max="35" width="11.5" bestFit="1" customWidth="1"/>
+    <col min="36" max="36" width="10.83203125" bestFit="1" customWidth="1"/>
+    <col min="37" max="37" width="11.83203125" customWidth="1"/>
+    <col min="38" max="38" width="16.1640625" bestFit="1" customWidth="1"/>
+    <col min="39" max="39" width="14.1640625" customWidth="1"/>
+    <col min="40" max="40" width="9.83203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:42" s="3" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:40" s="3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A1" s="12" t="s">
         <v>4</v>
       </c>
       <c r="B1" s="6" t="s">
         <v>27</v>
       </c>
-      <c r="C1" s="28" t="s">
+      <c r="C1" s="27" t="s">
         <v>33</v>
       </c>
-      <c r="D1" s="28"/>
+      <c r="D1" s="27"/>
       <c r="E1" s="6" t="s">
         <v>19</v>
       </c>
@@ -700,27 +703,27 @@
       <c r="G1" s="6" t="s">
         <v>34</v>
       </c>
-      <c r="H1" s="28" t="s">
+      <c r="H1" s="27" t="s">
         <v>45</v>
       </c>
-      <c r="I1" s="28"/>
-      <c r="J1" s="28"/>
-      <c r="K1" s="28" t="s">
+      <c r="I1" s="27"/>
+      <c r="J1" s="27"/>
+      <c r="K1" s="27" t="s">
         <v>35</v>
       </c>
-      <c r="L1" s="28"/>
-      <c r="M1" s="28"/>
-      <c r="N1" s="28" t="s">
+      <c r="L1" s="27"/>
+      <c r="M1" s="27"/>
+      <c r="N1" s="27" t="s">
         <v>48</v>
       </c>
-      <c r="O1" s="28"/>
+      <c r="O1" s="27"/>
       <c r="P1" s="5" t="s">
         <v>47</v>
       </c>
-      <c r="Q1" s="28" t="s">
+      <c r="Q1" s="27" t="s">
         <v>36</v>
       </c>
-      <c r="R1" s="28"/>
+      <c r="R1" s="27"/>
       <c r="S1" s="6" t="s">
         <v>37</v>
       </c>
@@ -736,40 +739,39 @@
       <c r="W1" s="4" t="s">
         <v>40</v>
       </c>
-      <c r="X1" s="29" t="s">
+      <c r="X1" s="28" t="s">
         <v>41</v>
       </c>
-      <c r="Y1" s="29"/>
-      <c r="Z1" s="29"/>
+      <c r="Y1" s="28"/>
+      <c r="Z1" s="28"/>
       <c r="AA1" s="15" t="s">
         <v>42</v>
       </c>
       <c r="AB1" s="15" t="s">
         <v>43</v>
       </c>
-      <c r="AC1" s="29" t="s">
+      <c r="AC1" s="28" t="s">
         <v>44</v>
       </c>
-      <c r="AD1" s="29"/>
-      <c r="AE1" s="29"/>
-      <c r="AF1" s="28" t="s">
+      <c r="AD1" s="28"/>
+      <c r="AE1" s="28"/>
+      <c r="AF1" s="27" t="s">
         <v>29</v>
       </c>
-      <c r="AG1" s="28"/>
-      <c r="AH1" s="28"/>
-      <c r="AI1" s="28" t="s">
+      <c r="AG1" s="27"/>
+      <c r="AH1" s="27"/>
+      <c r="AI1" s="27" t="s">
         <v>30</v>
       </c>
-      <c r="AJ1" s="28"/>
-      <c r="AK1" s="28"/>
-      <c r="AL1" s="28"/>
-      <c r="AM1" s="28" t="s">
+      <c r="AJ1" s="27"/>
+      <c r="AK1" s="27"/>
+      <c r="AL1" s="27"/>
+      <c r="AM1" s="27" t="s">
         <v>31</v>
       </c>
-      <c r="AN1" s="28"/>
-      <c r="AP1" s="26"/>
+      <c r="AN1" s="27"/>
     </row>
-    <row r="2" spans="1:42" s="7" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:40" s="7" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A2" s="12" t="s">
         <v>20</v>
       </c>
@@ -891,7 +893,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="3" spans="1:42" s="7" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:40" s="7" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A3" s="12" t="s">
         <v>11</v>
       </c>
@@ -1013,7 +1015,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="4" spans="1:42" s="7" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:40" s="7" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A4" s="12" t="s">
         <v>9</v>
       </c>
@@ -1135,7 +1137,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="5" spans="1:42" s="7" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:40" s="7" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A5" s="12" t="s">
         <v>10</v>
       </c>
@@ -1257,7 +1259,7 @@
         <v>8343</v>
       </c>
     </row>
-    <row r="6" spans="1:42" s="7" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:40" s="7" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A6" s="12" t="s">
         <v>21</v>
       </c>
@@ -1394,7 +1396,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:42" s="7" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:40" s="7" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A7" s="12" t="s">
         <v>0</v>
       </c>
@@ -1516,7 +1518,7 @@
         <v>522</v>
       </c>
     </row>
-    <row r="8" spans="1:42" s="8" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:40" s="8" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A8" s="13" t="s">
         <v>1</v>
       </c>
@@ -1638,7 +1640,7 @@
         <v>15000</v>
       </c>
     </row>
-    <row r="9" spans="1:42" s="7" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:40" s="7" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A9" s="12" t="s">
         <v>2</v>
       </c>
@@ -1760,7 +1762,7 @@
         <v>0.8</v>
       </c>
     </row>
-    <row r="10" spans="1:42" s="10" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:40" s="10" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A10" s="14" t="s">
         <v>3</v>
       </c>
@@ -1896,7 +1898,7 @@
         <v>94.337500000000006</v>
       </c>
     </row>
-    <row r="11" spans="1:42" s="7" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:40" s="7" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A11" s="12" t="s">
         <v>13</v>
       </c>
@@ -2018,144 +2020,144 @@
         <v>1.7</v>
       </c>
     </row>
-    <row r="12" spans="1:42" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A12" s="12" t="s">
         <v>32</v>
       </c>
-      <c r="B12" s="27" t="b">
-        <v>0</v>
-      </c>
-      <c r="C12" s="27" t="b">
-        <v>0</v>
-      </c>
-      <c r="D12" s="27" t="b">
-        <v>0</v>
-      </c>
-      <c r="E12" s="27" t="b">
-        <v>0</v>
-      </c>
-      <c r="F12" s="27" t="b">
-        <v>0</v>
-      </c>
-      <c r="G12" s="27" t="b">
-        <v>0</v>
-      </c>
-      <c r="H12" s="27" t="b">
-        <v>0</v>
-      </c>
-      <c r="I12" s="27" t="b">
-        <v>0</v>
-      </c>
-      <c r="J12" s="27" t="b">
-        <v>0</v>
-      </c>
-      <c r="K12" s="27" t="b">
-        <v>0</v>
-      </c>
-      <c r="L12" s="27" t="b">
-        <v>0</v>
-      </c>
-      <c r="M12" s="27" t="b">
-        <v>0</v>
-      </c>
-      <c r="N12" s="27" t="b">
-        <v>0</v>
-      </c>
-      <c r="O12" s="27" t="b">
-        <v>0</v>
-      </c>
-      <c r="P12" s="27" t="b">
-        <v>0</v>
-      </c>
-      <c r="Q12" s="27" t="b">
-        <v>0</v>
-      </c>
-      <c r="R12" s="27" t="b">
-        <v>0</v>
-      </c>
-      <c r="S12" s="27" t="b">
-        <v>0</v>
-      </c>
-      <c r="T12" s="27" t="b">
-        <v>0</v>
-      </c>
-      <c r="U12" s="27" t="b">
-        <v>0</v>
-      </c>
-      <c r="V12" s="27" t="b">
-        <v>0</v>
-      </c>
-      <c r="W12" s="27" t="b">
-        <v>0</v>
-      </c>
-      <c r="X12" s="27" t="b">
-        <v>0</v>
-      </c>
-      <c r="Y12" s="27" t="b">
-        <v>0</v>
-      </c>
-      <c r="Z12" s="27" t="b">
-        <v>0</v>
-      </c>
-      <c r="AA12" s="27" t="b">
-        <v>0</v>
-      </c>
-      <c r="AB12" s="27" t="b">
-        <v>0</v>
-      </c>
-      <c r="AC12" s="27" t="b">
-        <v>0</v>
-      </c>
-      <c r="AD12" s="27" t="b">
-        <v>0</v>
-      </c>
-      <c r="AE12" s="27" t="b">
-        <v>0</v>
-      </c>
-      <c r="AF12" s="27" t="b">
-        <v>0</v>
-      </c>
-      <c r="AG12" s="27" t="b">
-        <v>0</v>
-      </c>
-      <c r="AH12" s="27" t="b">
-        <v>0</v>
-      </c>
-      <c r="AI12" s="27" t="b">
-        <v>0</v>
-      </c>
-      <c r="AJ12" s="27" t="b">
-        <v>0</v>
-      </c>
-      <c r="AK12" s="27" t="b">
-        <v>0</v>
-      </c>
-      <c r="AL12" s="27" t="b">
-        <v>0</v>
-      </c>
-      <c r="AM12" s="27" t="b">
-        <v>0</v>
-      </c>
-      <c r="AN12" s="27" t="b">
+      <c r="B12" s="26" t="b">
+        <v>0</v>
+      </c>
+      <c r="C12" s="26" t="b">
+        <v>0</v>
+      </c>
+      <c r="D12" s="26" t="b">
+        <v>0</v>
+      </c>
+      <c r="E12" s="26" t="b">
+        <v>0</v>
+      </c>
+      <c r="F12" s="26" t="b">
+        <v>0</v>
+      </c>
+      <c r="G12" s="26" t="b">
+        <v>0</v>
+      </c>
+      <c r="H12" s="26" t="b">
+        <v>0</v>
+      </c>
+      <c r="I12" s="26" t="b">
+        <v>0</v>
+      </c>
+      <c r="J12" s="26" t="b">
+        <v>0</v>
+      </c>
+      <c r="K12" s="26" t="b">
+        <v>0</v>
+      </c>
+      <c r="L12" s="26" t="b">
+        <v>0</v>
+      </c>
+      <c r="M12" s="26" t="b">
+        <v>0</v>
+      </c>
+      <c r="N12" s="26" t="b">
+        <v>0</v>
+      </c>
+      <c r="O12" s="26" t="b">
+        <v>0</v>
+      </c>
+      <c r="P12" s="26" t="b">
+        <v>0</v>
+      </c>
+      <c r="Q12" s="26" t="b">
+        <v>0</v>
+      </c>
+      <c r="R12" s="26" t="b">
+        <v>0</v>
+      </c>
+      <c r="S12" s="26" t="b">
+        <v>0</v>
+      </c>
+      <c r="T12" s="26" t="b">
+        <v>0</v>
+      </c>
+      <c r="U12" s="26" t="b">
+        <v>0</v>
+      </c>
+      <c r="V12" s="26" t="b">
+        <v>0</v>
+      </c>
+      <c r="W12" s="26" t="b">
+        <v>0</v>
+      </c>
+      <c r="X12" s="26" t="b">
+        <v>0</v>
+      </c>
+      <c r="Y12" s="26" t="b">
+        <v>0</v>
+      </c>
+      <c r="Z12" s="26" t="b">
+        <v>0</v>
+      </c>
+      <c r="AA12" s="26" t="b">
+        <v>0</v>
+      </c>
+      <c r="AB12" s="26" t="b">
+        <v>0</v>
+      </c>
+      <c r="AC12" s="26" t="b">
+        <v>0</v>
+      </c>
+      <c r="AD12" s="26" t="b">
+        <v>0</v>
+      </c>
+      <c r="AE12" s="26" t="b">
+        <v>0</v>
+      </c>
+      <c r="AF12" s="26" t="b">
+        <v>0</v>
+      </c>
+      <c r="AG12" s="26" t="b">
+        <v>0</v>
+      </c>
+      <c r="AH12" s="26" t="b">
+        <v>0</v>
+      </c>
+      <c r="AI12" s="26" t="b">
+        <v>0</v>
+      </c>
+      <c r="AJ12" s="26" t="b">
+        <v>0</v>
+      </c>
+      <c r="AK12" s="26" t="b">
+        <v>0</v>
+      </c>
+      <c r="AL12" s="26" t="b">
+        <v>0</v>
+      </c>
+      <c r="AM12" s="26" t="b">
+        <v>0</v>
+      </c>
+      <c r="AN12" s="26" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A22" s="1"/>
     </row>
-    <row r="23" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A23" s="1"/>
     </row>
-    <row r="24" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A24" s="1"/>
     </row>
-    <row r="25" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A25" s="1"/>
     </row>
-    <row r="26" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A26" s="1"/>
     </row>
-    <row r="27" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A27" s="1"/>
     </row>
   </sheetData>
@@ -2177,16 +2179,16 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="C28" sqref="C28"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="8.77734375" customWidth="1"/>
+    <col min="1" max="1" width="8.83203125" customWidth="1"/>
   </cols>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2194,16 +2196,16 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:B3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="B28" sqref="B28"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>18</v>
       </c>
@@ -2211,7 +2213,7 @@
         <v>0.74570000000000003</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>26</v>
       </c>

</xml_diff>

<commit_message>
implement system factories in sugarcane to ethanol biorefinery, update analysis in cornstover and lipidcane to get plots, remove old files, update tests for new biosteam version
</commit_message>
<xml_diff>
--- a/BioSTEAM 2.x.x/biorefineries/cornstover/_humbird2011.xlsx
+++ b/BioSTEAM 2.x.x/biorefineries/cornstover/_humbird2011.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23426"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23530"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/733a0933307f0df0/Code/Bioindustrial-Park/BioSTEAM 2.x.x/biorefineries/cornstover/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="4" documentId="11_93738BBF658B224CE52DD40E9AAED54DBB468F57" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{B3335E70-828E-4AE4-8630-8A898F79D784}"/>
+  <xr:revisionPtr revIDLastSave="65" documentId="11_93738BBF658B224CE52DD40E9AAED54DBB468F57" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{7D86D35E-B81E-489C-9B67-8596242F0835}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="2820" windowWidth="20532" windowHeight="10980" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="14016" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="154" uniqueCount="51">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="165" uniqueCount="54">
   <si>
     <t>CEPCI</t>
   </si>
@@ -189,6 +189,15 @@
   </si>
   <si>
     <t>Lifetime (yr)</t>
+  </si>
+  <si>
+    <t>Sulfuric Acid Storage Tank</t>
+  </si>
+  <si>
+    <t>Tan k</t>
+  </si>
+  <si>
+    <t>Ammonia Storage Tank</t>
   </si>
 </sst>
 </file>
@@ -264,7 +273,7 @@
     <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="32">
+  <cellXfs count="34">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -346,6 +355,12 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -669,11 +684,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:AP27"/>
+  <dimension ref="A1:AR27"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="62" zoomScaleNormal="62" workbookViewId="0">
-      <pane xSplit="1" topLeftCell="AB1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="A13" sqref="A13"/>
+      <pane xSplit="1" topLeftCell="AL1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="AQ15" sqref="AQ15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -702,19 +717,23 @@
     <col min="38" max="38" width="16.109375" bestFit="1" customWidth="1"/>
     <col min="39" max="39" width="14.109375" customWidth="1"/>
     <col min="40" max="40" width="10.5546875" bestFit="1" customWidth="1"/>
+    <col min="41" max="41" width="13.33203125" customWidth="1"/>
+    <col min="42" max="42" width="17.6640625" customWidth="1"/>
+    <col min="43" max="43" width="23.77734375" bestFit="1" customWidth="1"/>
+    <col min="44" max="44" width="15.77734375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:42" s="3" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:44" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A1" s="12" t="s">
         <v>4</v>
       </c>
       <c r="B1" s="6" t="s">
         <v>27</v>
       </c>
-      <c r="C1" s="30" t="s">
+      <c r="C1" s="32" t="s">
         <v>33</v>
       </c>
-      <c r="D1" s="30"/>
+      <c r="D1" s="32"/>
       <c r="E1" s="6" t="s">
         <v>19</v>
       </c>
@@ -724,27 +743,27 @@
       <c r="G1" s="6" t="s">
         <v>34</v>
       </c>
-      <c r="H1" s="30" t="s">
+      <c r="H1" s="32" t="s">
         <v>45</v>
       </c>
-      <c r="I1" s="30"/>
-      <c r="J1" s="30"/>
-      <c r="K1" s="30" t="s">
+      <c r="I1" s="32"/>
+      <c r="J1" s="32"/>
+      <c r="K1" s="32" t="s">
         <v>35</v>
       </c>
-      <c r="L1" s="30"/>
-      <c r="M1" s="30"/>
-      <c r="N1" s="30" t="s">
+      <c r="L1" s="32"/>
+      <c r="M1" s="32"/>
+      <c r="N1" s="32" t="s">
         <v>48</v>
       </c>
-      <c r="O1" s="30"/>
+      <c r="O1" s="32"/>
       <c r="P1" s="5" t="s">
         <v>47</v>
       </c>
-      <c r="Q1" s="30" t="s">
+      <c r="Q1" s="32" t="s">
         <v>36</v>
       </c>
-      <c r="R1" s="30"/>
+      <c r="R1" s="32"/>
       <c r="S1" s="6" t="s">
         <v>37</v>
       </c>
@@ -760,40 +779,47 @@
       <c r="W1" s="4" t="s">
         <v>40</v>
       </c>
-      <c r="X1" s="31" t="s">
+      <c r="X1" s="33" t="s">
         <v>41</v>
       </c>
-      <c r="Y1" s="31"/>
-      <c r="Z1" s="31"/>
+      <c r="Y1" s="33"/>
+      <c r="Z1" s="33"/>
       <c r="AA1" s="15" t="s">
         <v>42</v>
       </c>
       <c r="AB1" s="15" t="s">
         <v>43</v>
       </c>
-      <c r="AC1" s="31" t="s">
+      <c r="AC1" s="33" t="s">
         <v>44</v>
       </c>
-      <c r="AD1" s="31"/>
-      <c r="AE1" s="31"/>
-      <c r="AF1" s="30" t="s">
+      <c r="AD1" s="33"/>
+      <c r="AE1" s="33"/>
+      <c r="AF1" s="32" t="s">
         <v>29</v>
       </c>
-      <c r="AG1" s="30"/>
-      <c r="AH1" s="30"/>
-      <c r="AI1" s="30" t="s">
+      <c r="AG1" s="32"/>
+      <c r="AH1" s="32"/>
+      <c r="AI1" s="32" t="s">
         <v>30</v>
       </c>
-      <c r="AJ1" s="30"/>
-      <c r="AK1" s="30"/>
-      <c r="AL1" s="30"/>
-      <c r="AM1" s="30" t="s">
+      <c r="AJ1" s="32"/>
+      <c r="AK1" s="32"/>
+      <c r="AL1" s="32"/>
+      <c r="AM1" s="32" t="s">
         <v>31</v>
       </c>
-      <c r="AN1" s="30"/>
-      <c r="AP1" s="26"/>
+      <c r="AN1" s="32"/>
+      <c r="AO1" s="32" t="s">
+        <v>51</v>
+      </c>
+      <c r="AP1" s="32"/>
+      <c r="AQ1" s="26" t="s">
+        <v>53</v>
+      </c>
+      <c r="AR1" s="26"/>
     </row>
-    <row r="2" spans="1:42" s="7" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:44" s="7" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A2" s="12" t="s">
         <v>20</v>
       </c>
@@ -914,8 +940,17 @@
       <c r="AN2" s="24" t="s">
         <v>16</v>
       </c>
+      <c r="AO2" s="7" t="s">
+        <v>52</v>
+      </c>
+      <c r="AP2" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="AQ2" s="7" t="s">
+        <v>8</v>
+      </c>
     </row>
-    <row r="3" spans="1:42" s="7" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:44" s="7" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A3" s="12" t="s">
         <v>11</v>
       </c>
@@ -1036,8 +1071,17 @@
       <c r="AN3" s="24" t="s">
         <v>6</v>
       </c>
+      <c r="AO3" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="AP3" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="AQ3" s="7" t="s">
+        <v>6</v>
+      </c>
     </row>
-    <row r="4" spans="1:42" s="7" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:44" s="7" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A4" s="12" t="s">
         <v>9</v>
       </c>
@@ -1158,8 +1202,18 @@
       <c r="AN4" s="25" t="s">
         <v>7</v>
       </c>
+      <c r="AO4" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="AP4" s="30" t="s">
+        <v>7</v>
+      </c>
+      <c r="AQ4" s="30" t="s">
+        <v>7</v>
+      </c>
+      <c r="AR4" s="30"/>
     </row>
-    <row r="5" spans="1:42" s="7" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:44" s="7" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A5" s="12" t="s">
         <v>10</v>
       </c>
@@ -1280,8 +1334,18 @@
       <c r="AN5" s="24">
         <v>8343</v>
       </c>
+      <c r="AO5" s="7">
+        <v>1981</v>
+      </c>
+      <c r="AP5" s="7">
+        <v>1981</v>
+      </c>
+      <c r="AQ5" s="7">
+        <v>1171</v>
+      </c>
+      <c r="AR5" s="30"/>
     </row>
-    <row r="6" spans="1:42" s="7" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:44" s="7" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A6" s="12" t="s">
         <v>21</v>
       </c>
@@ -1417,8 +1481,17 @@
       <c r="AN6" s="24" t="b">
         <v>0</v>
       </c>
+      <c r="AO6" s="7" t="b">
+        <v>0</v>
+      </c>
+      <c r="AP6" s="7" t="b">
+        <v>0</v>
+      </c>
+      <c r="AQ6" s="7" t="b">
+        <v>0</v>
+      </c>
     </row>
-    <row r="7" spans="1:42" s="7" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:44" s="7" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A7" s="12" t="s">
         <v>0</v>
       </c>
@@ -1539,8 +1612,17 @@
       <c r="AN7" s="24">
         <v>522</v>
       </c>
+      <c r="AO7" s="30">
+        <v>522</v>
+      </c>
+      <c r="AP7" s="7">
+        <v>522</v>
+      </c>
+      <c r="AQ7" s="7">
+        <v>522</v>
+      </c>
     </row>
-    <row r="8" spans="1:42" s="8" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:44" s="8" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A8" s="13" t="s">
         <v>1</v>
       </c>
@@ -1661,8 +1743,17 @@
       <c r="AN8" s="8">
         <v>15000</v>
       </c>
+      <c r="AO8" s="8">
+        <v>96000</v>
+      </c>
+      <c r="AP8" s="8">
+        <v>7493</v>
+      </c>
+      <c r="AQ8" s="8">
+        <v>196000</v>
+      </c>
     </row>
-    <row r="9" spans="1:42" s="7" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:44" s="7" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A9" s="12" t="s">
         <v>2</v>
       </c>
@@ -1783,8 +1874,17 @@
       <c r="AN9" s="24">
         <v>0.8</v>
       </c>
+      <c r="AO9" s="7">
+        <v>0.7</v>
+      </c>
+      <c r="AP9" s="7">
+        <v>0.8</v>
+      </c>
+      <c r="AQ9" s="7">
+        <v>0.7</v>
+      </c>
     </row>
-    <row r="10" spans="1:42" s="10" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:44" s="10" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A10" s="14" t="s">
         <v>3</v>
       </c>
@@ -1919,8 +2019,17 @@
         <f>125*0.7547</f>
         <v>94.337500000000006</v>
       </c>
+      <c r="AO10" s="10">
+        <v>0</v>
+      </c>
+      <c r="AP10" s="10">
+        <v>0.5</v>
+      </c>
+      <c r="AQ10" s="10">
+        <v>0</v>
+      </c>
     </row>
-    <row r="11" spans="1:42" s="7" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:44" s="7" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A11" s="12" t="s">
         <v>13</v>
       </c>
@@ -2041,8 +2150,17 @@
       <c r="AN11" s="24">
         <v>1.7</v>
       </c>
+      <c r="AO11" s="7">
+        <v>1.5</v>
+      </c>
+      <c r="AP11" s="7">
+        <v>2.2999999999999998</v>
+      </c>
+      <c r="AQ11" s="7">
+        <v>2</v>
+      </c>
     </row>
-    <row r="12" spans="1:42" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:44" x14ac:dyDescent="0.3">
       <c r="A12" s="12" t="s">
         <v>32</v>
       </c>
@@ -2163,8 +2281,18 @@
       <c r="AN12" s="27" t="b">
         <v>0</v>
       </c>
+      <c r="AO12" s="31" t="b">
+        <v>0</v>
+      </c>
+      <c r="AP12" s="31" t="b">
+        <v>0</v>
+      </c>
+      <c r="AQ12" s="31" t="b">
+        <v>0</v>
+      </c>
+      <c r="AR12" s="31"/>
     </row>
-    <row r="13" spans="1:42" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:44" x14ac:dyDescent="0.3">
       <c r="A13" s="29" t="s">
         <v>50</v>
       </c>
@@ -2285,6 +2413,16 @@
       <c r="AN13" s="28" t="b">
         <v>0</v>
       </c>
+      <c r="AO13" s="31" t="b">
+        <v>0</v>
+      </c>
+      <c r="AP13" s="31" t="b">
+        <v>0</v>
+      </c>
+      <c r="AQ13" s="31" t="b">
+        <v>0</v>
+      </c>
+      <c r="AR13" s="31"/>
     </row>
     <row r="22" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A22" s="1"/>
@@ -2305,7 +2443,8 @@
       <c r="A27" s="1"/>
     </row>
   </sheetData>
-  <mergeCells count="10">
+  <mergeCells count="11">
+    <mergeCell ref="AO1:AP1"/>
     <mergeCell ref="AI1:AL1"/>
     <mergeCell ref="AM1:AN1"/>
     <mergeCell ref="C1:D1"/>

</xml_diff>

<commit_message>
refactor code and update results
</commit_message>
<xml_diff>
--- a/BioSTEAM 2.x.x/biorefineries/cornstover/_humbird2011.xlsx
+++ b/BioSTEAM 2.x.x/biorefineries/cornstover/_humbird2011.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/733a0933307f0df0/Code/Bioindustrial-Park/BioSTEAM 2.x.x/biorefineries/cornstover/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="65" documentId="11_93738BBF658B224CE52DD40E9AAED54DBB468F57" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{7D86D35E-B81E-489C-9B67-8596242F0835}"/>
+  <xr:revisionPtr revIDLastSave="68" documentId="11_93738BBF658B224CE52DD40E9AAED54DBB468F57" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{86F5A0B3-8C5D-4190-9FDC-6A6C5332F3BA}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="14016" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2508" yWindow="2820" windowWidth="20532" windowHeight="10980" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -182,9 +182,6 @@
     <t>Mixer-Ammonia mixer</t>
   </si>
   <si>
-    <t>Ammonia addition tank</t>
-  </si>
-  <si>
     <t>Bag unloader</t>
   </si>
   <si>
@@ -198,6 +195,9 @@
   </si>
   <si>
     <t>Ammonia Storage Tank</t>
+  </si>
+  <si>
+    <t>MixTank-Ammonia addition tank</t>
   </si>
 </sst>
 </file>
@@ -687,8 +687,8 @@
   <dimension ref="A1:AR27"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="62" zoomScaleNormal="62" workbookViewId="0">
-      <pane xSplit="1" topLeftCell="AL1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="AQ15" sqref="AQ15"/>
+      <pane xSplit="1" topLeftCell="H1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="N6" sqref="N6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -754,7 +754,7 @@
       <c r="L1" s="32"/>
       <c r="M1" s="32"/>
       <c r="N1" s="32" t="s">
-        <v>48</v>
+        <v>53</v>
       </c>
       <c r="O1" s="32"/>
       <c r="P1" s="5" t="s">
@@ -811,11 +811,11 @@
       </c>
       <c r="AN1" s="32"/>
       <c r="AO1" s="32" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="AP1" s="32"/>
       <c r="AQ1" s="26" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="AR1" s="26"/>
     </row>
@@ -932,7 +932,7 @@
         <v>15</v>
       </c>
       <c r="AL2" s="7" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="AM2" s="24" t="s">
         <v>8</v>
@@ -941,7 +941,7 @@
         <v>16</v>
       </c>
       <c r="AO2" s="7" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="AP2" s="7" t="s">
         <v>16</v>
@@ -2294,7 +2294,7 @@
     </row>
     <row r="13" spans="1:44" x14ac:dyDescent="0.3">
       <c r="A13" s="29" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B13" s="28" t="b">
         <v>0</v>

</xml_diff>

<commit_message>
continue work on lipidcane2g
</commit_message>
<xml_diff>
--- a/BioSTEAM 2.x.x/biorefineries/cornstover/_humbird2011.xlsx
+++ b/BioSTEAM 2.x.x/biorefineries/cornstover/_humbird2011.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23530"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23801"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/733a0933307f0df0/Code/Bioindustrial-Park/BioSTEAM 2.x.x/biorefineries/cornstover/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="68" documentId="11_93738BBF658B224CE52DD40E9AAED54DBB468F57" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{86F5A0B3-8C5D-4190-9FDC-6A6C5332F3BA}"/>
+  <xr:revisionPtr revIDLastSave="76" documentId="11_93738BBF658B224CE52DD40E9AAED54DBB468F57" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{8FBAE52F-AB7D-4B05-99DD-98324BB7C5D0}"/>
   <bookViews>
-    <workbookView xWindow="2508" yWindow="2820" windowWidth="20532" windowHeight="10980" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView minimized="1" xWindow="2508" yWindow="2820" windowWidth="20532" windowHeight="10980" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="165" uniqueCount="54">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="166" uniqueCount="55">
   <si>
     <t>CEPCI</t>
   </si>
@@ -125,15 +125,6 @@
     <t>Heat exchanger</t>
   </si>
   <si>
-    <t>CSL Tank</t>
-  </si>
-  <si>
-    <t>DAP Tank</t>
-  </si>
-  <si>
-    <t>Fire Water Tank</t>
-  </si>
-  <si>
     <t>Number</t>
   </si>
   <si>
@@ -198,6 +189,18 @@
   </si>
   <si>
     <t>MixTank-Ammonia addition tank</t>
+  </si>
+  <si>
+    <t>CSL Storage Tank</t>
+  </si>
+  <si>
+    <t>DAP Storage Tank</t>
+  </si>
+  <si>
+    <t>Fire Water Storage Tank</t>
+  </si>
+  <si>
+    <t>Lower bound</t>
   </si>
 </sst>
 </file>
@@ -273,7 +276,7 @@
     <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="34">
+  <cellXfs count="36">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -355,6 +358,12 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -684,11 +693,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:AR27"/>
+  <dimension ref="A1:AR28"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="62" zoomScaleNormal="62" workbookViewId="0">
-      <pane xSplit="1" topLeftCell="H1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="N6" sqref="N6"/>
+      <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="AN13" sqref="AN13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -707,12 +716,11 @@
     <col min="27" max="27" width="29.44140625" customWidth="1"/>
     <col min="28" max="28" width="32.109375" customWidth="1"/>
     <col min="29" max="29" width="24.6640625" bestFit="1" customWidth="1"/>
-    <col min="30" max="30" width="9.88671875" bestFit="1" customWidth="1"/>
-    <col min="31" max="31" width="10.21875" customWidth="1"/>
-    <col min="32" max="32" width="9.88671875" bestFit="1" customWidth="1"/>
-    <col min="34" max="34" width="9.88671875" bestFit="1" customWidth="1"/>
+    <col min="30" max="32" width="10.88671875" bestFit="1" customWidth="1"/>
+    <col min="33" max="33" width="9.77734375" bestFit="1" customWidth="1"/>
+    <col min="34" max="34" width="10.5546875" bestFit="1" customWidth="1"/>
     <col min="35" max="35" width="11.5546875" bestFit="1" customWidth="1"/>
-    <col min="36" max="36" width="10.88671875" bestFit="1" customWidth="1"/>
+    <col min="36" max="36" width="9.77734375" bestFit="1" customWidth="1"/>
     <col min="37" max="37" width="11.77734375" customWidth="1"/>
     <col min="38" max="38" width="16.109375" bestFit="1" customWidth="1"/>
     <col min="39" max="39" width="14.109375" customWidth="1"/>
@@ -730,10 +738,10 @@
       <c r="B1" s="6" t="s">
         <v>27</v>
       </c>
-      <c r="C1" s="32" t="s">
-        <v>33</v>
-      </c>
-      <c r="D1" s="32"/>
+      <c r="C1" s="34" t="s">
+        <v>30</v>
+      </c>
+      <c r="D1" s="34"/>
       <c r="E1" s="6" t="s">
         <v>19</v>
       </c>
@@ -741,81 +749,81 @@
         <v>5</v>
       </c>
       <c r="G1" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="H1" s="34" t="s">
+        <v>42</v>
+      </c>
+      <c r="I1" s="34"/>
+      <c r="J1" s="34"/>
+      <c r="K1" s="34" t="s">
+        <v>32</v>
+      </c>
+      <c r="L1" s="34"/>
+      <c r="M1" s="34"/>
+      <c r="N1" s="34" t="s">
+        <v>50</v>
+      </c>
+      <c r="O1" s="34"/>
+      <c r="P1" s="5" t="s">
+        <v>44</v>
+      </c>
+      <c r="Q1" s="34" t="s">
+        <v>33</v>
+      </c>
+      <c r="R1" s="34"/>
+      <c r="S1" s="6" t="s">
         <v>34</v>
       </c>
-      <c r="H1" s="32" t="s">
-        <v>45</v>
-      </c>
-      <c r="I1" s="32"/>
-      <c r="J1" s="32"/>
-      <c r="K1" s="32" t="s">
+      <c r="T1" s="6" t="s">
+        <v>43</v>
+      </c>
+      <c r="U1" s="6" t="s">
         <v>35</v>
       </c>
-      <c r="L1" s="32"/>
-      <c r="M1" s="32"/>
-      <c r="N1" s="32" t="s">
+      <c r="V1" s="6" t="s">
+        <v>36</v>
+      </c>
+      <c r="W1" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="X1" s="35" t="s">
+        <v>38</v>
+      </c>
+      <c r="Y1" s="35"/>
+      <c r="Z1" s="35"/>
+      <c r="AA1" s="15" t="s">
+        <v>39</v>
+      </c>
+      <c r="AB1" s="15" t="s">
+        <v>40</v>
+      </c>
+      <c r="AC1" s="35" t="s">
+        <v>41</v>
+      </c>
+      <c r="AD1" s="35"/>
+      <c r="AE1" s="35"/>
+      <c r="AF1" s="34" t="s">
+        <v>51</v>
+      </c>
+      <c r="AG1" s="34"/>
+      <c r="AH1" s="34"/>
+      <c r="AI1" s="34" t="s">
+        <v>52</v>
+      </c>
+      <c r="AJ1" s="34"/>
+      <c r="AK1" s="34"/>
+      <c r="AL1" s="34"/>
+      <c r="AM1" s="34" t="s">
         <v>53</v>
       </c>
-      <c r="O1" s="32"/>
-      <c r="P1" s="5" t="s">
+      <c r="AN1" s="34"/>
+      <c r="AO1" s="34" t="s">
         <v>47</v>
       </c>
-      <c r="Q1" s="32" t="s">
-        <v>36</v>
-      </c>
-      <c r="R1" s="32"/>
-      <c r="S1" s="6" t="s">
-        <v>37</v>
-      </c>
-      <c r="T1" s="6" t="s">
-        <v>46</v>
-      </c>
-      <c r="U1" s="6" t="s">
-        <v>38</v>
-      </c>
-      <c r="V1" s="6" t="s">
-        <v>39</v>
-      </c>
-      <c r="W1" s="4" t="s">
-        <v>40</v>
-      </c>
-      <c r="X1" s="33" t="s">
-        <v>41</v>
-      </c>
-      <c r="Y1" s="33"/>
-      <c r="Z1" s="33"/>
-      <c r="AA1" s="15" t="s">
-        <v>42</v>
-      </c>
-      <c r="AB1" s="15" t="s">
-        <v>43</v>
-      </c>
-      <c r="AC1" s="33" t="s">
-        <v>44</v>
-      </c>
-      <c r="AD1" s="33"/>
-      <c r="AE1" s="33"/>
-      <c r="AF1" s="32" t="s">
-        <v>29</v>
-      </c>
-      <c r="AG1" s="32"/>
-      <c r="AH1" s="32"/>
-      <c r="AI1" s="32" t="s">
-        <v>30</v>
-      </c>
-      <c r="AJ1" s="32"/>
-      <c r="AK1" s="32"/>
-      <c r="AL1" s="32"/>
-      <c r="AM1" s="32" t="s">
-        <v>31</v>
-      </c>
-      <c r="AN1" s="32"/>
-      <c r="AO1" s="32" t="s">
-        <v>50</v>
-      </c>
-      <c r="AP1" s="32"/>
+      <c r="AP1" s="34"/>
       <c r="AQ1" s="26" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="AR1" s="26"/>
     </row>
@@ -932,7 +940,7 @@
         <v>15</v>
       </c>
       <c r="AL2" s="7" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="AM2" s="24" t="s">
         <v>8</v>
@@ -941,7 +949,7 @@
         <v>16</v>
       </c>
       <c r="AO2" s="7" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="AP2" s="7" t="s">
         <v>16</v>
@@ -1345,1072 +1353,1086 @@
       </c>
       <c r="AR5" s="30"/>
     </row>
-    <row r="6" spans="1:44" s="7" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:44" s="32" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A6" s="12" t="s">
-        <v>21</v>
-      </c>
-      <c r="B6" s="7" t="b">
-        <f>FALSE</f>
-        <v>0</v>
-      </c>
-      <c r="C6" s="7" t="b">
-        <f>FALSE</f>
-        <v>0</v>
-      </c>
-      <c r="D6" s="7" t="b">
-        <f>FALSE</f>
-        <v>0</v>
-      </c>
-      <c r="E6" s="7" t="b">
-        <f>FALSE</f>
-        <v>0</v>
-      </c>
-      <c r="F6" s="7" t="b">
-        <f>FALSE</f>
-        <v>0</v>
-      </c>
-      <c r="G6" s="7" t="b">
-        <f>FALSE</f>
-        <v>0</v>
-      </c>
-      <c r="H6" s="7" t="b">
-        <f>FALSE</f>
-        <v>0</v>
-      </c>
-      <c r="I6" s="7" t="b">
-        <f>FALSE</f>
-        <v>0</v>
-      </c>
-      <c r="J6" s="7" t="b">
-        <f>FALSE</f>
-        <v>0</v>
-      </c>
-      <c r="K6" s="7" t="b">
-        <f>FALSE</f>
-        <v>0</v>
-      </c>
-      <c r="L6" s="7" t="b">
-        <f>FALSE</f>
-        <v>0</v>
-      </c>
-      <c r="M6" s="7" t="b">
-        <f>FALSE</f>
-        <v>0</v>
-      </c>
-      <c r="N6" s="7" t="b">
-        <f>FALSE</f>
-        <v>0</v>
-      </c>
-      <c r="O6" s="7" t="b">
-        <f>FALSE</f>
-        <v>0</v>
-      </c>
-      <c r="P6" s="7" t="b">
-        <f>FALSE</f>
-        <v>0</v>
-      </c>
-      <c r="Q6" s="7" t="b">
-        <v>0</v>
-      </c>
-      <c r="R6" s="7" t="b">
-        <v>0</v>
-      </c>
-      <c r="S6" s="7" t="b">
-        <v>0</v>
-      </c>
-      <c r="T6" s="4" t="b">
-        <v>0</v>
-      </c>
-      <c r="U6" s="4" t="b">
-        <v>0</v>
-      </c>
-      <c r="V6" s="4" t="b">
-        <v>0</v>
-      </c>
-      <c r="W6" s="4" t="b">
-        <v>0</v>
-      </c>
-      <c r="X6" s="4" t="b">
-        <v>0</v>
-      </c>
-      <c r="Y6" s="4" t="b">
-        <v>0</v>
-      </c>
-      <c r="Z6" s="4" t="b">
-        <v>0</v>
-      </c>
-      <c r="AA6" s="4" t="b">
-        <v>0</v>
-      </c>
-      <c r="AB6" s="4" t="b">
-        <v>0</v>
-      </c>
-      <c r="AC6" s="7" t="b">
-        <v>0</v>
-      </c>
-      <c r="AD6" s="7" t="b">
-        <v>0</v>
-      </c>
-      <c r="AE6" s="7" t="b">
-        <v>0</v>
-      </c>
-      <c r="AF6" s="19" t="b">
-        <v>0</v>
-      </c>
-      <c r="AG6" s="19" t="b">
-        <v>0</v>
-      </c>
-      <c r="AH6" s="19" t="b">
-        <v>0</v>
-      </c>
-      <c r="AI6" s="23" t="b">
-        <v>0</v>
-      </c>
-      <c r="AJ6" s="23" t="b">
-        <v>0</v>
-      </c>
-      <c r="AK6" s="23" t="b">
-        <v>0</v>
-      </c>
-      <c r="AL6" s="23" t="b">
-        <v>0</v>
-      </c>
-      <c r="AM6" s="24" t="b">
-        <v>0</v>
-      </c>
-      <c r="AN6" s="24" t="b">
-        <v>0</v>
-      </c>
-      <c r="AO6" s="7" t="b">
-        <v>0</v>
-      </c>
-      <c r="AP6" s="7" t="b">
-        <v>0</v>
-      </c>
-      <c r="AQ6" s="7" t="b">
+        <v>54</v>
+      </c>
+      <c r="B6" s="32" t="b">
+        <f>FALSE</f>
+        <v>0</v>
+      </c>
+      <c r="C6" s="32" t="b">
+        <f>FALSE</f>
+        <v>0</v>
+      </c>
+      <c r="D6" s="32" t="b">
+        <f>FALSE</f>
+        <v>0</v>
+      </c>
+      <c r="E6" s="32" t="b">
+        <f>FALSE</f>
+        <v>0</v>
+      </c>
+      <c r="F6" s="32" t="b">
+        <f>FALSE</f>
+        <v>0</v>
+      </c>
+      <c r="G6" s="32" t="b">
+        <f>FALSE</f>
+        <v>0</v>
+      </c>
+      <c r="H6" s="32" t="b">
+        <f>FALSE</f>
+        <v>0</v>
+      </c>
+      <c r="I6" s="32" t="b">
+        <f>FALSE</f>
+        <v>0</v>
+      </c>
+      <c r="J6" s="32" t="b">
+        <f>FALSE</f>
+        <v>0</v>
+      </c>
+      <c r="K6" s="32" t="b">
+        <f>FALSE</f>
+        <v>0</v>
+      </c>
+      <c r="L6" s="32" t="b">
+        <f>FALSE</f>
+        <v>0</v>
+      </c>
+      <c r="M6" s="32" t="b">
+        <f>FALSE</f>
+        <v>0</v>
+      </c>
+      <c r="N6" s="32" t="b">
+        <f>FALSE</f>
+        <v>0</v>
+      </c>
+      <c r="O6" s="32" t="b">
+        <f>FALSE</f>
+        <v>0</v>
+      </c>
+      <c r="P6" s="32" t="b">
+        <f>FALSE</f>
+        <v>0</v>
+      </c>
+      <c r="Q6" s="32" t="b">
+        <v>0</v>
+      </c>
+      <c r="R6" s="32" t="b">
+        <v>0</v>
+      </c>
+      <c r="S6" s="32" t="b">
+        <v>0</v>
+      </c>
+      <c r="T6" s="33" t="b">
+        <v>0</v>
+      </c>
+      <c r="U6" s="33" t="b">
+        <v>0</v>
+      </c>
+      <c r="V6" s="33" t="b">
+        <v>0</v>
+      </c>
+      <c r="W6" s="33" t="b">
+        <v>0</v>
+      </c>
+      <c r="X6" s="33" t="b">
+        <v>0</v>
+      </c>
+      <c r="Y6" s="33" t="b">
+        <v>0</v>
+      </c>
+      <c r="Z6" s="33" t="b">
+        <v>0</v>
+      </c>
+      <c r="AA6" s="33" t="b">
+        <v>0</v>
+      </c>
+      <c r="AB6" s="33" t="b">
+        <v>0</v>
+      </c>
+      <c r="AC6" s="32" t="b">
+        <v>0</v>
+      </c>
+      <c r="AD6" s="32" t="b">
+        <v>0</v>
+      </c>
+      <c r="AE6" s="32" t="b">
+        <v>0</v>
+      </c>
+      <c r="AF6" s="32" t="b">
+        <v>0</v>
+      </c>
+      <c r="AG6" s="32" t="b">
+        <v>0</v>
+      </c>
+      <c r="AH6" s="32" t="b">
+        <v>0</v>
+      </c>
+      <c r="AI6" s="32" t="b">
+        <v>0</v>
+      </c>
+      <c r="AJ6" s="32" t="b">
+        <v>0</v>
+      </c>
+      <c r="AK6" s="32" t="b">
+        <v>0</v>
+      </c>
+      <c r="AL6" s="32" t="b">
+        <v>0</v>
+      </c>
+      <c r="AM6" s="32" t="b">
+        <v>0</v>
+      </c>
+      <c r="AN6" s="32" t="b">
+        <v>0</v>
+      </c>
+      <c r="AO6" s="32" t="b">
+        <v>0</v>
+      </c>
+      <c r="AP6" s="32" t="b">
+        <v>0</v>
+      </c>
+      <c r="AQ6" s="32" t="b">
         <v>0</v>
       </c>
     </row>
     <row r="7" spans="1:44" s="7" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A7" s="12" t="s">
-        <v>0</v>
-      </c>
-      <c r="B7" s="7">
-        <v>522</v>
-      </c>
-      <c r="C7" s="7">
+        <v>21</v>
+      </c>
+      <c r="B7" s="7" t="b">
+        <f>FALSE</f>
+        <v>0</v>
+      </c>
+      <c r="C7" s="7" t="b">
+        <f>FALSE</f>
+        <v>0</v>
+      </c>
+      <c r="D7" s="7" t="b">
+        <f>FALSE</f>
+        <v>0</v>
+      </c>
+      <c r="E7" s="7" t="b">
+        <f>FALSE</f>
+        <v>0</v>
+      </c>
+      <c r="F7" s="7" t="b">
+        <f>FALSE</f>
+        <v>0</v>
+      </c>
+      <c r="G7" s="7" t="b">
+        <f>FALSE</f>
+        <v>0</v>
+      </c>
+      <c r="H7" s="7" t="b">
+        <f>FALSE</f>
+        <v>0</v>
+      </c>
+      <c r="I7" s="7" t="b">
+        <f>FALSE</f>
+        <v>0</v>
+      </c>
+      <c r="J7" s="7" t="b">
+        <f>FALSE</f>
+        <v>0</v>
+      </c>
+      <c r="K7" s="7" t="b">
+        <f>FALSE</f>
+        <v>0</v>
+      </c>
+      <c r="L7" s="7" t="b">
+        <f>FALSE</f>
+        <v>0</v>
+      </c>
+      <c r="M7" s="7" t="b">
+        <f>FALSE</f>
+        <v>0</v>
+      </c>
+      <c r="N7" s="7" t="b">
+        <f>FALSE</f>
+        <v>0</v>
+      </c>
+      <c r="O7" s="7" t="b">
+        <f>FALSE</f>
+        <v>0</v>
+      </c>
+      <c r="P7" s="7" t="b">
+        <f>FALSE</f>
+        <v>0</v>
+      </c>
+      <c r="Q7" s="7" t="b">
+        <v>0</v>
+      </c>
+      <c r="R7" s="7" t="b">
+        <v>0</v>
+      </c>
+      <c r="S7" s="7" t="b">
+        <v>0</v>
+      </c>
+      <c r="T7" s="4" t="b">
+        <v>0</v>
+      </c>
+      <c r="U7" s="4" t="b">
+        <v>0</v>
+      </c>
+      <c r="V7" s="4" t="b">
+        <v>0</v>
+      </c>
+      <c r="W7" s="4" t="b">
+        <v>0</v>
+      </c>
+      <c r="X7" s="4" t="b">
+        <v>0</v>
+      </c>
+      <c r="Y7" s="4" t="b">
+        <v>0</v>
+      </c>
+      <c r="Z7" s="4" t="b">
+        <v>0</v>
+      </c>
+      <c r="AA7" s="4" t="b">
+        <v>0</v>
+      </c>
+      <c r="AB7" s="4" t="b">
+        <v>0</v>
+      </c>
+      <c r="AC7" s="7" t="b">
+        <v>0</v>
+      </c>
+      <c r="AD7" s="7" t="b">
+        <v>0</v>
+      </c>
+      <c r="AE7" s="7" t="b">
+        <v>0</v>
+      </c>
+      <c r="AF7" s="19" t="b">
+        <v>0</v>
+      </c>
+      <c r="AG7" s="19" t="b">
+        <v>0</v>
+      </c>
+      <c r="AH7" s="19" t="b">
+        <v>0</v>
+      </c>
+      <c r="AI7" s="23" t="b">
+        <v>0</v>
+      </c>
+      <c r="AJ7" s="23" t="b">
+        <v>0</v>
+      </c>
+      <c r="AK7" s="23" t="b">
+        <v>0</v>
+      </c>
+      <c r="AL7" s="23" t="b">
+        <v>0</v>
+      </c>
+      <c r="AM7" s="24" t="b">
+        <v>0</v>
+      </c>
+      <c r="AN7" s="24" t="b">
+        <v>0</v>
+      </c>
+      <c r="AO7" s="7" t="b">
+        <v>0</v>
+      </c>
+      <c r="AP7" s="7" t="b">
+        <v>0</v>
+      </c>
+      <c r="AQ7" s="7" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:44" s="7" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A8" s="12" t="s">
+        <v>0</v>
+      </c>
+      <c r="B8" s="7">
+        <v>522</v>
+      </c>
+      <c r="C8" s="7">
         <v>551</v>
       </c>
-      <c r="D7" s="7">
-        <v>522</v>
-      </c>
-      <c r="E7" s="7">
-        <v>522</v>
-      </c>
-      <c r="F7" s="7">
-        <v>522</v>
-      </c>
-      <c r="G7" s="7">
+      <c r="D8" s="7">
+        <v>522</v>
+      </c>
+      <c r="E8" s="7">
+        <v>522</v>
+      </c>
+      <c r="F8" s="7">
+        <v>522</v>
+      </c>
+      <c r="G8" s="7">
         <v>551</v>
       </c>
-      <c r="H7" s="7">
-        <v>522</v>
-      </c>
-      <c r="I7" s="7">
-        <v>522</v>
-      </c>
-      <c r="J7" s="7">
-        <v>522</v>
-      </c>
-      <c r="K7" s="7">
-        <v>522</v>
-      </c>
-      <c r="L7" s="7">
+      <c r="H8" s="7">
+        <v>522</v>
+      </c>
+      <c r="I8" s="7">
+        <v>522</v>
+      </c>
+      <c r="J8" s="7">
+        <v>522</v>
+      </c>
+      <c r="K8" s="7">
+        <v>522</v>
+      </c>
+      <c r="L8" s="7">
         <v>551</v>
       </c>
-      <c r="M7" s="7">
-        <v>522</v>
-      </c>
-      <c r="N7" s="7">
-        <v>522</v>
-      </c>
-      <c r="O7" s="7">
-        <v>522</v>
-      </c>
-      <c r="P7" s="4">
-        <v>522</v>
-      </c>
-      <c r="Q7" s="7">
-        <v>522</v>
-      </c>
-      <c r="R7" s="7">
-        <v>522</v>
-      </c>
-      <c r="S7" s="7">
+      <c r="M8" s="7">
+        <v>522</v>
+      </c>
+      <c r="N8" s="7">
+        <v>522</v>
+      </c>
+      <c r="O8" s="7">
+        <v>522</v>
+      </c>
+      <c r="P8" s="4">
+        <v>522</v>
+      </c>
+      <c r="Q8" s="7">
+        <v>522</v>
+      </c>
+      <c r="R8" s="7">
+        <v>522</v>
+      </c>
+      <c r="S8" s="7">
         <v>551</v>
       </c>
-      <c r="T7" s="4">
-        <v>522</v>
-      </c>
-      <c r="U7" s="4">
-        <v>522</v>
-      </c>
-      <c r="V7" s="4">
-        <v>522</v>
-      </c>
-      <c r="W7" s="4">
-        <v>522</v>
-      </c>
-      <c r="X7" s="4">
-        <v>522</v>
-      </c>
-      <c r="Y7" s="4">
-        <v>522</v>
-      </c>
-      <c r="Z7" s="4">
-        <v>522</v>
-      </c>
-      <c r="AA7" s="4">
-        <v>522</v>
-      </c>
-      <c r="AB7" s="4">
-        <v>522</v>
-      </c>
-      <c r="AC7" s="7">
-        <v>522</v>
-      </c>
-      <c r="AD7" s="7">
-        <v>522</v>
-      </c>
-      <c r="AE7" s="7">
-        <v>522</v>
-      </c>
-      <c r="AF7" s="7">
-        <v>522</v>
-      </c>
-      <c r="AG7" s="19">
-        <v>522</v>
-      </c>
-      <c r="AH7" s="19">
-        <v>522</v>
-      </c>
-      <c r="AI7" s="23">
-        <v>522</v>
-      </c>
-      <c r="AJ7" s="23">
-        <v>522</v>
-      </c>
-      <c r="AK7" s="23">
-        <v>522</v>
-      </c>
-      <c r="AL7" s="23">
-        <v>522</v>
-      </c>
-      <c r="AM7" s="24">
-        <v>522</v>
-      </c>
-      <c r="AN7" s="24">
-        <v>522</v>
-      </c>
-      <c r="AO7" s="30">
-        <v>522</v>
-      </c>
-      <c r="AP7" s="7">
-        <v>522</v>
-      </c>
-      <c r="AQ7" s="7">
+      <c r="T8" s="4">
+        <v>522</v>
+      </c>
+      <c r="U8" s="4">
+        <v>522</v>
+      </c>
+      <c r="V8" s="4">
+        <v>522</v>
+      </c>
+      <c r="W8" s="4">
+        <v>522</v>
+      </c>
+      <c r="X8" s="4">
+        <v>522</v>
+      </c>
+      <c r="Y8" s="4">
+        <v>522</v>
+      </c>
+      <c r="Z8" s="4">
+        <v>522</v>
+      </c>
+      <c r="AA8" s="4">
+        <v>522</v>
+      </c>
+      <c r="AB8" s="4">
+        <v>522</v>
+      </c>
+      <c r="AC8" s="7">
+        <v>522</v>
+      </c>
+      <c r="AD8" s="7">
+        <v>522</v>
+      </c>
+      <c r="AE8" s="7">
+        <v>522</v>
+      </c>
+      <c r="AF8" s="7">
+        <v>522</v>
+      </c>
+      <c r="AG8" s="19">
+        <v>522</v>
+      </c>
+      <c r="AH8" s="19">
+        <v>522</v>
+      </c>
+      <c r="AI8" s="23">
+        <v>522</v>
+      </c>
+      <c r="AJ8" s="23">
+        <v>522</v>
+      </c>
+      <c r="AK8" s="23">
+        <v>522</v>
+      </c>
+      <c r="AL8" s="23">
+        <v>522</v>
+      </c>
+      <c r="AM8" s="24">
+        <v>522</v>
+      </c>
+      <c r="AN8" s="24">
+        <v>522</v>
+      </c>
+      <c r="AO8" s="30">
+        <v>522</v>
+      </c>
+      <c r="AP8" s="7">
+        <v>522</v>
+      </c>
+      <c r="AQ8" s="7">
         <v>522</v>
       </c>
     </row>
-    <row r="8" spans="1:44" s="8" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="13" t="s">
+    <row r="9" spans="1:44" s="8" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A9" s="13" t="s">
         <v>1</v>
       </c>
-      <c r="B8" s="8">
+      <c r="B9" s="8">
         <v>13329690</v>
       </c>
-      <c r="C8" s="8">
+      <c r="C9" s="8">
         <v>6210</v>
       </c>
-      <c r="D8" s="8">
+      <c r="D9" s="8">
         <v>8000</v>
       </c>
-      <c r="E8" s="8">
+      <c r="E9" s="8">
         <v>6000</v>
       </c>
-      <c r="F8" s="8">
+      <c r="F9" s="8">
         <v>19812400</v>
       </c>
-      <c r="G8" s="8">
+      <c r="G9" s="8">
         <v>25365</v>
       </c>
-      <c r="H8" s="8">
+      <c r="H9" s="8">
         <v>511000</v>
       </c>
-      <c r="I8" s="8">
+      <c r="I9" s="8">
         <v>30000</v>
       </c>
-      <c r="J8" s="8">
+      <c r="J9" s="8">
         <v>90000</v>
       </c>
-      <c r="K8" s="8">
+      <c r="K9" s="8">
         <v>203000</v>
       </c>
-      <c r="L8" s="8">
+      <c r="L9" s="8">
         <v>17480</v>
       </c>
-      <c r="M8" s="8">
+      <c r="M9" s="8">
         <v>90000</v>
       </c>
-      <c r="N8" s="8">
+      <c r="N9" s="8">
         <v>236000</v>
       </c>
-      <c r="O8" s="8">
+      <c r="O9" s="8">
         <v>21900</v>
       </c>
-      <c r="P8" s="9">
+      <c r="P9" s="9">
         <v>5000</v>
       </c>
-      <c r="Q8" s="8">
-        <v>0</v>
-      </c>
-      <c r="R8" s="8">
-        <v>0</v>
-      </c>
-      <c r="S8" s="8">
+      <c r="Q9" s="8">
+        <v>0</v>
+      </c>
+      <c r="R9" s="8">
+        <v>0</v>
+      </c>
+      <c r="S9" s="8">
         <v>92000</v>
       </c>
-      <c r="T8" s="8">
+      <c r="T9" s="8">
         <v>34000</v>
       </c>
-      <c r="U8" s="4">
+      <c r="U9" s="4">
         <v>22500</v>
       </c>
-      <c r="V8" s="21">
-        <v>0</v>
-      </c>
-      <c r="W8" s="8">
+      <c r="V9" s="21">
+        <v>0</v>
+      </c>
+      <c r="W9" s="8">
         <v>35000000</v>
       </c>
-      <c r="X8" s="8">
+      <c r="X9" s="8">
         <v>8200</v>
       </c>
-      <c r="Y8" s="8">
+      <c r="Y9" s="8">
         <v>439000</v>
       </c>
-      <c r="Z8" s="8">
+      <c r="Z9" s="8">
         <v>31800</v>
       </c>
-      <c r="AA8" s="8">
+      <c r="AA9" s="8">
         <v>85000</v>
       </c>
-      <c r="AB8" s="8">
+      <c r="AB9" s="8">
         <v>109000</v>
       </c>
-      <c r="AC8" s="8">
+      <c r="AC9" s="8">
         <v>636000</v>
       </c>
-      <c r="AD8" s="8">
+      <c r="AD9" s="8">
         <v>26800</v>
       </c>
-      <c r="AE8" s="8">
+      <c r="AE9" s="8">
         <v>68300</v>
       </c>
-      <c r="AF8" s="8">
+      <c r="AF9" s="8">
         <v>70000</v>
       </c>
-      <c r="AG8" s="8">
+      <c r="AG9" s="8">
         <v>3000</v>
       </c>
-      <c r="AH8" s="8">
+      <c r="AH9" s="8">
         <v>21200</v>
       </c>
-      <c r="AI8" s="8">
+      <c r="AI9" s="8">
         <v>102000</v>
       </c>
-      <c r="AJ8" s="8">
+      <c r="AJ9" s="8">
         <v>3000</v>
       </c>
-      <c r="AK8" s="8">
+      <c r="AK9" s="8">
         <v>9800</v>
       </c>
-      <c r="AL8" s="8">
+      <c r="AL9" s="8">
         <v>30000</v>
       </c>
-      <c r="AM8" s="8">
+      <c r="AM9" s="8">
         <v>803000</v>
       </c>
-      <c r="AN8" s="8">
+      <c r="AN9" s="8">
         <v>15000</v>
       </c>
-      <c r="AO8" s="8">
+      <c r="AO9" s="8">
         <v>96000</v>
       </c>
-      <c r="AP8" s="8">
+      <c r="AP9" s="8">
         <v>7493</v>
       </c>
-      <c r="AQ8" s="8">
+      <c r="AQ9" s="8">
         <v>196000</v>
       </c>
     </row>
-    <row r="9" spans="1:44" s="7" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="12" t="s">
+    <row r="10" spans="1:44" s="7" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A10" s="12" t="s">
         <v>2</v>
       </c>
-      <c r="B9" s="7">
+      <c r="B10" s="7">
         <v>0.6</v>
       </c>
-      <c r="C9" s="7">
+      <c r="C10" s="7">
         <v>0.7</v>
       </c>
-      <c r="D9" s="7">
+      <c r="D10" s="7">
         <v>0.8</v>
       </c>
-      <c r="E9" s="7">
+      <c r="E10" s="7">
         <v>0.5</v>
       </c>
-      <c r="F9" s="7">
+      <c r="F10" s="7">
         <v>0.6</v>
       </c>
-      <c r="G9" s="7">
+      <c r="G10" s="7">
         <v>0.8</v>
       </c>
-      <c r="H9" s="7">
+      <c r="H10" s="7">
         <v>0.7</v>
       </c>
-      <c r="I9" s="7">
+      <c r="I10" s="7">
         <v>0.8</v>
       </c>
-      <c r="J9" s="7">
+      <c r="J10" s="7">
         <v>0.5</v>
       </c>
-      <c r="K9" s="7">
+      <c r="K10" s="7">
         <v>0.7</v>
       </c>
-      <c r="L9" s="7">
+      <c r="L10" s="7">
         <v>0.8</v>
       </c>
-      <c r="M9" s="7">
+      <c r="M10" s="7">
         <v>0.5</v>
       </c>
-      <c r="N9" s="7">
+      <c r="N10" s="7">
         <v>0.7</v>
       </c>
-      <c r="O9" s="7">
+      <c r="O10" s="7">
         <v>0.5</v>
       </c>
-      <c r="P9" s="4">
+      <c r="P10" s="4">
         <v>0.5</v>
       </c>
-      <c r="Q9" s="7">
+      <c r="Q10" s="7">
         <v>0.5</v>
       </c>
-      <c r="R9" s="7">
+      <c r="R10" s="7">
         <v>0.7</v>
       </c>
-      <c r="S9" s="7">
+      <c r="S10" s="7">
         <v>0.7</v>
       </c>
-      <c r="T9" s="4">
+      <c r="T10" s="4">
         <v>0.7</v>
       </c>
-      <c r="U9" s="4">
+      <c r="U10" s="4">
         <v>0.8</v>
       </c>
-      <c r="V9" s="4">
+      <c r="V10" s="4">
         <v>0.8</v>
       </c>
-      <c r="W9" s="7">
+      <c r="W10" s="7">
         <v>0.7</v>
       </c>
-      <c r="X9" s="7">
+      <c r="X10" s="7">
         <v>0.8</v>
       </c>
-      <c r="Y9" s="7">
+      <c r="Y10" s="7">
         <v>0.7</v>
       </c>
-      <c r="Z9" s="7">
+      <c r="Z10" s="7">
         <v>0.5</v>
       </c>
-      <c r="AA9" s="4">
+      <c r="AA10" s="4">
         <v>0.7</v>
       </c>
-      <c r="AB9" s="4">
+      <c r="AB10" s="4">
         <v>0.5</v>
       </c>
-      <c r="AC9" s="7">
+      <c r="AC10" s="7">
         <v>0.7</v>
       </c>
-      <c r="AD9" s="7">
+      <c r="AD10" s="7">
         <v>0.8</v>
       </c>
-      <c r="AE9" s="7">
+      <c r="AE10" s="7">
         <v>0.5</v>
       </c>
-      <c r="AF9" s="7">
+      <c r="AF10" s="7">
         <v>0.7</v>
       </c>
-      <c r="AG9" s="7">
+      <c r="AG10" s="7">
         <v>0.8</v>
       </c>
-      <c r="AH9" s="7">
+      <c r="AH10" s="7">
         <v>0.5</v>
       </c>
-      <c r="AI9" s="23">
+      <c r="AI10" s="23">
         <v>0.7</v>
       </c>
-      <c r="AJ9" s="23">
+      <c r="AJ10" s="23">
         <v>0.8</v>
       </c>
-      <c r="AK9" s="23">
+      <c r="AK10" s="23">
         <v>0.5</v>
       </c>
-      <c r="AL9" s="23">
+      <c r="AL10" s="23">
         <v>0.6</v>
       </c>
-      <c r="AM9" s="24">
+      <c r="AM10" s="24">
         <v>0.7</v>
       </c>
-      <c r="AN9" s="24">
+      <c r="AN10" s="24">
         <v>0.8</v>
       </c>
-      <c r="AO9" s="7">
+      <c r="AO10" s="7">
         <v>0.7</v>
       </c>
-      <c r="AP9" s="7">
+      <c r="AP10" s="7">
         <v>0.8</v>
       </c>
-      <c r="AQ9" s="7">
+      <c r="AQ10" s="7">
         <v>0.7</v>
       </c>
     </row>
-    <row r="10" spans="1:44" s="10" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="14" t="s">
+    <row r="11" spans="1:44" s="10" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A11" s="14" t="s">
         <v>3</v>
       </c>
-      <c r="B10" s="10">
+      <c r="B11" s="10">
         <v>783</v>
       </c>
-      <c r="C10" s="10">
-        <v>0</v>
-      </c>
-      <c r="D10" s="10">
+      <c r="C11" s="10">
+        <v>0</v>
+      </c>
+      <c r="D11" s="10">
         <v>1</v>
       </c>
-      <c r="E10" s="10">
-        <v>0</v>
-      </c>
-      <c r="F10" s="10">
+      <c r="E11" s="10">
+        <v>0</v>
+      </c>
+      <c r="F11" s="10">
         <v>5290</v>
       </c>
-      <c r="G10" s="10">
+      <c r="G11" s="10">
         <f>125*Sheet2!B1</f>
         <v>93.212500000000006</v>
       </c>
-      <c r="H10" s="10">
-        <v>0</v>
-      </c>
-      <c r="I10" s="10">
+      <c r="H11" s="10">
+        <v>0</v>
+      </c>
+      <c r="I11" s="10">
         <v>55.9</v>
       </c>
-      <c r="J10" s="10">
+      <c r="J11" s="10">
         <v>170</v>
       </c>
-      <c r="K10" s="10">
-        <v>0</v>
-      </c>
-      <c r="L10" s="10">
+      <c r="K11" s="10">
+        <v>0</v>
+      </c>
+      <c r="L11" s="10">
         <v>55.9</v>
       </c>
-      <c r="M10" s="10">
+      <c r="M11" s="10">
         <v>170</v>
       </c>
-      <c r="N10" s="10">
-        <v>0</v>
-      </c>
-      <c r="O10" s="10">
+      <c r="N11" s="10">
+        <v>0</v>
+      </c>
+      <c r="O11" s="10">
         <f>10*Sheet2!B1</f>
         <v>7.4570000000000007</v>
       </c>
-      <c r="P10" s="11">
-        <v>0</v>
-      </c>
-      <c r="Q10" s="10">
+      <c r="P11" s="11">
+        <v>0</v>
+      </c>
+      <c r="Q11" s="10">
         <f>20*Sheet2!B1</f>
         <v>14.914000000000001</v>
       </c>
-      <c r="R10" s="10">
-        <v>0</v>
-      </c>
-      <c r="S10" s="10">
-        <v>0</v>
-      </c>
-      <c r="T10" s="10">
-        <v>0</v>
-      </c>
-      <c r="U10" s="4">
+      <c r="R11" s="10">
+        <v>0</v>
+      </c>
+      <c r="S11" s="10">
+        <v>0</v>
+      </c>
+      <c r="T11" s="10">
+        <v>0</v>
+      </c>
+      <c r="U11" s="4">
         <f>100*Sheet2!B$1</f>
         <v>74.570000000000007</v>
       </c>
-      <c r="V10" s="4">
+      <c r="V11" s="4">
         <f>60*Sheet2!B$1</f>
         <v>44.742000000000004</v>
       </c>
-      <c r="W10" s="10">
-        <v>0</v>
-      </c>
-      <c r="X10" s="10">
+      <c r="W11" s="10">
+        <v>0</v>
+      </c>
+      <c r="X11" s="10">
         <f>10*0.7457</f>
         <v>7.4570000000000007</v>
       </c>
-      <c r="Y10" s="10">
-        <v>0</v>
-      </c>
-      <c r="Z10" s="10">
+      <c r="Y11" s="10">
+        <v>0</v>
+      </c>
+      <c r="Z11" s="10">
         <f>15*0.7547</f>
         <v>11.320500000000001</v>
       </c>
-      <c r="AA10" s="10">
-        <v>0</v>
-      </c>
-      <c r="AB10" s="10">
+      <c r="AA11" s="10">
+        <v>0</v>
+      </c>
+      <c r="AB11" s="10">
         <f>100*0.7457</f>
         <v>74.570000000000007</v>
       </c>
-      <c r="AC10" s="10">
-        <v>0</v>
-      </c>
-      <c r="AD10" s="10">
+      <c r="AC11" s="10">
+        <v>0</v>
+      </c>
+      <c r="AD11" s="10">
         <f>125*0.7457</f>
         <v>93.212500000000006</v>
       </c>
-      <c r="AE10" s="10">
+      <c r="AE11" s="10">
         <f>20*0.7457</f>
         <v>14.914000000000001</v>
       </c>
-      <c r="AF10" s="10">
-        <v>0</v>
-      </c>
-      <c r="AG10" s="10">
+      <c r="AF11" s="10">
+        <v>0</v>
+      </c>
+      <c r="AG11" s="10">
         <f>0.5*Sheet2!B1</f>
         <v>0.37285000000000001</v>
       </c>
-      <c r="AH10" s="10">
+      <c r="AH11" s="10">
         <v>7.4569999999999999</v>
       </c>
-      <c r="AI10" s="10">
-        <v>0</v>
-      </c>
-      <c r="AJ10" s="10">
+      <c r="AI11" s="10">
+        <v>0</v>
+      </c>
+      <c r="AJ11" s="10">
         <f>0.5*0.7547</f>
         <v>0.37735000000000002</v>
       </c>
-      <c r="AK10" s="10">
+      <c r="AK11" s="10">
         <f>5.5*0.7457</f>
         <v>4.1013500000000001</v>
       </c>
-      <c r="AL10" s="10">
-        <v>0</v>
-      </c>
-      <c r="AM10" s="10">
-        <v>0</v>
-      </c>
-      <c r="AN10" s="10">
+      <c r="AL11" s="10">
+        <v>0</v>
+      </c>
+      <c r="AM11" s="10">
+        <v>0</v>
+      </c>
+      <c r="AN11" s="10">
         <f>125*0.7547</f>
         <v>94.337500000000006</v>
       </c>
-      <c r="AO10" s="10">
-        <v>0</v>
-      </c>
-      <c r="AP10" s="10">
+      <c r="AO11" s="10">
+        <v>0</v>
+      </c>
+      <c r="AP11" s="10">
         <v>0.5</v>
       </c>
-      <c r="AQ10" s="10">
+      <c r="AQ11" s="10">
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:44" s="7" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="12" t="s">
+    <row r="12" spans="1:44" s="7" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A12" s="12" t="s">
         <v>13</v>
       </c>
-      <c r="B11" s="7">
+      <c r="B12" s="7">
         <v>1.7</v>
       </c>
-      <c r="C11" s="7">
+      <c r="C12" s="7">
         <v>2</v>
       </c>
-      <c r="D11" s="7">
+      <c r="D12" s="7">
         <v>2.2999999999999998</v>
       </c>
-      <c r="E11" s="7">
+      <c r="E12" s="7">
         <v>1</v>
       </c>
-      <c r="F11" s="7">
+      <c r="F12" s="7">
         <v>2.2000000000000002</v>
       </c>
-      <c r="G11" s="7">
+      <c r="G12" s="7">
         <v>2.2999999999999998</v>
       </c>
-      <c r="H11" s="7">
+      <c r="H12" s="7">
         <v>2</v>
       </c>
-      <c r="I11" s="7">
+      <c r="I12" s="7">
         <v>1.7</v>
       </c>
-      <c r="J11" s="7">
+      <c r="J12" s="7">
         <v>1.5</v>
       </c>
-      <c r="K11" s="7">
+      <c r="K12" s="7">
         <v>2</v>
       </c>
-      <c r="L11" s="7">
+      <c r="L12" s="7">
         <v>1.7</v>
       </c>
-      <c r="M11" s="7">
+      <c r="M12" s="7">
         <v>1.5</v>
       </c>
-      <c r="N11" s="7">
+      <c r="N12" s="7">
         <v>2</v>
       </c>
-      <c r="O11" s="7">
+      <c r="O12" s="7">
         <v>1.5</v>
       </c>
-      <c r="P11" s="4">
+      <c r="P12" s="4">
         <v>1</v>
       </c>
-      <c r="Q11" s="7">
+      <c r="Q12" s="7">
         <v>1.5</v>
       </c>
-      <c r="R11" s="7">
+      <c r="R12" s="7">
         <v>2</v>
       </c>
-      <c r="S11" s="7">
+      <c r="S12" s="7">
         <v>2.2000000000000002</v>
       </c>
-      <c r="T11" s="4">
+      <c r="T12" s="4">
         <v>2.2000000000000002</v>
       </c>
-      <c r="U11" s="4">
+      <c r="U12" s="4">
         <v>2.2999999999999998</v>
       </c>
-      <c r="V11" s="4">
+      <c r="V12" s="4">
         <v>2.2999999999999998</v>
       </c>
-      <c r="W11" s="7">
+      <c r="W12" s="7">
         <v>1.7</v>
       </c>
-      <c r="X11" s="7">
+      <c r="X12" s="7">
         <v>2.2999999999999998</v>
       </c>
-      <c r="Y11" s="7">
+      <c r="Y12" s="7">
         <v>1.8</v>
       </c>
-      <c r="Z11" s="7">
+      <c r="Z12" s="7">
         <v>1.5</v>
       </c>
-      <c r="AA11" s="7">
+      <c r="AA12" s="7">
         <v>2.2000000000000002</v>
       </c>
-      <c r="AB11" s="7">
+      <c r="AB12" s="7">
         <v>1.7</v>
       </c>
-      <c r="AC11" s="7">
+      <c r="AC12" s="7">
         <v>1.8</v>
       </c>
-      <c r="AD11" s="7">
+      <c r="AD12" s="7">
         <v>2.2999999999999998</v>
       </c>
-      <c r="AE11" s="7">
+      <c r="AE12" s="7">
         <v>1.5</v>
       </c>
-      <c r="AF11" s="7">
+      <c r="AF12" s="7">
         <v>2.6</v>
       </c>
-      <c r="AG11" s="7">
+      <c r="AG12" s="7">
         <v>3.1</v>
       </c>
-      <c r="AH11" s="7">
+      <c r="AH12" s="7">
         <v>1.5</v>
       </c>
-      <c r="AI11" s="23">
+      <c r="AI12" s="23">
         <v>1.8</v>
       </c>
-      <c r="AJ11" s="23">
+      <c r="AJ12" s="23">
         <v>3.1</v>
       </c>
-      <c r="AK11" s="23">
+      <c r="AK12" s="23">
         <v>1.5</v>
       </c>
-      <c r="AL11" s="23">
+      <c r="AL12" s="23">
         <v>1.7</v>
       </c>
-      <c r="AM11" s="24">
+      <c r="AM12" s="24">
         <v>1.8</v>
       </c>
-      <c r="AN11" s="24">
+      <c r="AN12" s="24">
         <v>1.7</v>
       </c>
-      <c r="AO11" s="7">
+      <c r="AO12" s="7">
         <v>1.5</v>
       </c>
-      <c r="AP11" s="7">
+      <c r="AP12" s="7">
         <v>2.2999999999999998</v>
       </c>
-      <c r="AQ11" s="7">
+      <c r="AQ12" s="7">
         <v>2</v>
       </c>
-    </row>
-    <row r="12" spans="1:44" x14ac:dyDescent="0.3">
-      <c r="A12" s="12" t="s">
-        <v>32</v>
-      </c>
-      <c r="B12" s="27" t="b">
-        <v>0</v>
-      </c>
-      <c r="C12" s="27" t="b">
-        <v>0</v>
-      </c>
-      <c r="D12" s="27" t="b">
-        <v>0</v>
-      </c>
-      <c r="E12" s="27" t="b">
-        <v>0</v>
-      </c>
-      <c r="F12" s="27" t="b">
-        <v>0</v>
-      </c>
-      <c r="G12" s="27" t="b">
-        <v>0</v>
-      </c>
-      <c r="H12" s="27" t="b">
-        <v>0</v>
-      </c>
-      <c r="I12" s="27" t="b">
-        <v>0</v>
-      </c>
-      <c r="J12" s="27" t="b">
-        <v>0</v>
-      </c>
-      <c r="K12" s="27" t="b">
-        <v>0</v>
-      </c>
-      <c r="L12" s="27" t="b">
-        <v>0</v>
-      </c>
-      <c r="M12" s="27" t="b">
-        <v>0</v>
-      </c>
-      <c r="N12" s="27" t="b">
-        <v>0</v>
-      </c>
-      <c r="O12" s="27" t="b">
-        <v>0</v>
-      </c>
-      <c r="P12" s="27" t="b">
-        <v>0</v>
-      </c>
-      <c r="Q12" s="27" t="b">
-        <v>0</v>
-      </c>
-      <c r="R12" s="27" t="b">
-        <v>0</v>
-      </c>
-      <c r="S12" s="27" t="b">
-        <v>0</v>
-      </c>
-      <c r="T12" s="27" t="b">
-        <v>0</v>
-      </c>
-      <c r="U12" s="27" t="b">
-        <v>0</v>
-      </c>
-      <c r="V12" s="27" t="b">
-        <v>0</v>
-      </c>
-      <c r="W12" s="27" t="b">
-        <v>0</v>
-      </c>
-      <c r="X12" s="27" t="b">
-        <v>0</v>
-      </c>
-      <c r="Y12" s="27" t="b">
-        <v>0</v>
-      </c>
-      <c r="Z12" s="27" t="b">
-        <v>0</v>
-      </c>
-      <c r="AA12" s="27" t="b">
-        <v>0</v>
-      </c>
-      <c r="AB12" s="27" t="b">
-        <v>0</v>
-      </c>
-      <c r="AC12" s="27" t="b">
-        <v>0</v>
-      </c>
-      <c r="AD12" s="27" t="b">
-        <v>0</v>
-      </c>
-      <c r="AE12" s="27" t="b">
-        <v>0</v>
-      </c>
-      <c r="AF12" s="27" t="b">
-        <v>0</v>
-      </c>
-      <c r="AG12" s="27" t="b">
-        <v>0</v>
-      </c>
-      <c r="AH12" s="27" t="b">
-        <v>0</v>
-      </c>
-      <c r="AI12" s="27" t="b">
-        <v>0</v>
-      </c>
-      <c r="AJ12" s="27" t="b">
-        <v>0</v>
-      </c>
-      <c r="AK12" s="27" t="b">
-        <v>0</v>
-      </c>
-      <c r="AL12" s="27" t="b">
-        <v>0</v>
-      </c>
-      <c r="AM12" s="27" t="b">
-        <v>0</v>
-      </c>
-      <c r="AN12" s="27" t="b">
-        <v>0</v>
-      </c>
-      <c r="AO12" s="31" t="b">
-        <v>0</v>
-      </c>
-      <c r="AP12" s="31" t="b">
-        <v>0</v>
-      </c>
-      <c r="AQ12" s="31" t="b">
-        <v>0</v>
-      </c>
-      <c r="AR12" s="31"/>
     </row>
     <row r="13" spans="1:44" x14ac:dyDescent="0.3">
-      <c r="A13" s="29" t="s">
-        <v>49</v>
-      </c>
-      <c r="B13" s="28" t="b">
-        <v>0</v>
-      </c>
-      <c r="C13" s="28" t="b">
-        <v>0</v>
-      </c>
-      <c r="D13" s="28" t="b">
-        <v>0</v>
-      </c>
-      <c r="E13" s="28" t="b">
-        <v>0</v>
-      </c>
-      <c r="F13" s="28" t="b">
-        <v>0</v>
-      </c>
-      <c r="G13" s="28" t="b">
-        <v>0</v>
-      </c>
-      <c r="H13" s="28" t="b">
-        <v>0</v>
-      </c>
-      <c r="I13" s="28" t="b">
-        <v>0</v>
-      </c>
-      <c r="J13" s="28" t="b">
-        <v>0</v>
-      </c>
-      <c r="K13" s="28" t="b">
-        <v>0</v>
-      </c>
-      <c r="L13" s="28" t="b">
-        <v>0</v>
-      </c>
-      <c r="M13" s="28" t="b">
-        <v>0</v>
-      </c>
-      <c r="N13" s="28" t="b">
-        <v>0</v>
-      </c>
-      <c r="O13" s="28" t="b">
-        <v>0</v>
-      </c>
-      <c r="P13" s="28" t="b">
-        <v>0</v>
-      </c>
-      <c r="Q13" s="28" t="b">
-        <v>0</v>
-      </c>
-      <c r="R13" s="28" t="b">
-        <v>0</v>
-      </c>
-      <c r="S13" s="28" t="b">
-        <v>0</v>
-      </c>
-      <c r="T13" s="28" t="b">
-        <v>0</v>
-      </c>
-      <c r="U13" s="28" t="b">
-        <v>0</v>
-      </c>
-      <c r="V13" s="28" t="b">
-        <v>0</v>
-      </c>
-      <c r="W13" s="28" t="b">
-        <v>0</v>
-      </c>
-      <c r="X13" s="28" t="b">
-        <v>0</v>
-      </c>
-      <c r="Y13" s="28" t="b">
-        <v>0</v>
-      </c>
-      <c r="Z13" s="28" t="b">
-        <v>0</v>
-      </c>
-      <c r="AA13" s="28" t="b">
-        <v>0</v>
-      </c>
-      <c r="AB13" s="28" t="b">
-        <v>0</v>
-      </c>
-      <c r="AC13" s="28" t="b">
-        <v>0</v>
-      </c>
-      <c r="AD13" s="28" t="b">
-        <v>0</v>
-      </c>
-      <c r="AE13" s="28" t="b">
-        <v>0</v>
-      </c>
-      <c r="AF13" s="28" t="b">
-        <v>0</v>
-      </c>
-      <c r="AG13" s="28" t="b">
-        <v>0</v>
-      </c>
-      <c r="AH13" s="28" t="b">
-        <v>0</v>
-      </c>
-      <c r="AI13" s="28" t="b">
-        <v>0</v>
-      </c>
-      <c r="AJ13" s="28" t="b">
-        <v>0</v>
-      </c>
-      <c r="AK13" s="28" t="b">
-        <v>0</v>
-      </c>
-      <c r="AL13" s="28" t="b">
-        <v>0</v>
-      </c>
-      <c r="AM13" s="28" t="b">
-        <v>0</v>
-      </c>
-      <c r="AN13" s="28" t="b">
+      <c r="A13" s="12" t="s">
+        <v>29</v>
+      </c>
+      <c r="B13" s="27" t="b">
+        <v>0</v>
+      </c>
+      <c r="C13" s="27" t="b">
+        <v>0</v>
+      </c>
+      <c r="D13" s="27" t="b">
+        <v>0</v>
+      </c>
+      <c r="E13" s="27" t="b">
+        <v>0</v>
+      </c>
+      <c r="F13" s="27" t="b">
+        <v>0</v>
+      </c>
+      <c r="G13" s="27" t="b">
+        <v>0</v>
+      </c>
+      <c r="H13" s="27" t="b">
+        <v>0</v>
+      </c>
+      <c r="I13" s="27" t="b">
+        <v>0</v>
+      </c>
+      <c r="J13" s="27" t="b">
+        <v>0</v>
+      </c>
+      <c r="K13" s="27" t="b">
+        <v>0</v>
+      </c>
+      <c r="L13" s="27" t="b">
+        <v>0</v>
+      </c>
+      <c r="M13" s="27" t="b">
+        <v>0</v>
+      </c>
+      <c r="N13" s="27" t="b">
+        <v>0</v>
+      </c>
+      <c r="O13" s="27" t="b">
+        <v>0</v>
+      </c>
+      <c r="P13" s="27" t="b">
+        <v>0</v>
+      </c>
+      <c r="Q13" s="27" t="b">
+        <v>0</v>
+      </c>
+      <c r="R13" s="27" t="b">
+        <v>0</v>
+      </c>
+      <c r="S13" s="27" t="b">
+        <v>0</v>
+      </c>
+      <c r="T13" s="27" t="b">
+        <v>0</v>
+      </c>
+      <c r="U13" s="27" t="b">
+        <v>0</v>
+      </c>
+      <c r="V13" s="27" t="b">
+        <v>0</v>
+      </c>
+      <c r="W13" s="27" t="b">
+        <v>0</v>
+      </c>
+      <c r="X13" s="27" t="b">
+        <v>0</v>
+      </c>
+      <c r="Y13" s="27" t="b">
+        <v>0</v>
+      </c>
+      <c r="Z13" s="27" t="b">
+        <v>0</v>
+      </c>
+      <c r="AA13" s="27" t="b">
+        <v>0</v>
+      </c>
+      <c r="AB13" s="27" t="b">
+        <v>0</v>
+      </c>
+      <c r="AC13" s="27" t="b">
+        <v>0</v>
+      </c>
+      <c r="AD13" s="27" t="b">
+        <v>0</v>
+      </c>
+      <c r="AE13" s="27" t="b">
+        <v>0</v>
+      </c>
+      <c r="AF13" s="27" t="b">
+        <v>0</v>
+      </c>
+      <c r="AG13" s="27" t="b">
+        <v>0</v>
+      </c>
+      <c r="AH13" s="27" t="b">
+        <v>0</v>
+      </c>
+      <c r="AI13" s="27" t="b">
+        <v>0</v>
+      </c>
+      <c r="AJ13" s="27" t="b">
+        <v>0</v>
+      </c>
+      <c r="AK13" s="27" t="b">
+        <v>0</v>
+      </c>
+      <c r="AL13" s="27" t="b">
+        <v>0</v>
+      </c>
+      <c r="AM13" s="27" t="b">
+        <v>0</v>
+      </c>
+      <c r="AN13" s="27" t="b">
         <v>0</v>
       </c>
       <c r="AO13" s="31" t="b">
@@ -2424,8 +2446,137 @@
       </c>
       <c r="AR13" s="31"/>
     </row>
-    <row r="22" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A22" s="1"/>
+    <row r="14" spans="1:44" x14ac:dyDescent="0.3">
+      <c r="A14" s="29" t="s">
+        <v>46</v>
+      </c>
+      <c r="B14" s="28" t="b">
+        <v>0</v>
+      </c>
+      <c r="C14" s="28" t="b">
+        <v>0</v>
+      </c>
+      <c r="D14" s="28" t="b">
+        <v>0</v>
+      </c>
+      <c r="E14" s="28" t="b">
+        <v>0</v>
+      </c>
+      <c r="F14" s="28" t="b">
+        <v>0</v>
+      </c>
+      <c r="G14" s="28" t="b">
+        <v>0</v>
+      </c>
+      <c r="H14" s="28" t="b">
+        <v>0</v>
+      </c>
+      <c r="I14" s="28" t="b">
+        <v>0</v>
+      </c>
+      <c r="J14" s="28" t="b">
+        <v>0</v>
+      </c>
+      <c r="K14" s="28" t="b">
+        <v>0</v>
+      </c>
+      <c r="L14" s="28" t="b">
+        <v>0</v>
+      </c>
+      <c r="M14" s="28" t="b">
+        <v>0</v>
+      </c>
+      <c r="N14" s="28" t="b">
+        <v>0</v>
+      </c>
+      <c r="O14" s="28" t="b">
+        <v>0</v>
+      </c>
+      <c r="P14" s="28" t="b">
+        <v>0</v>
+      </c>
+      <c r="Q14" s="28" t="b">
+        <v>0</v>
+      </c>
+      <c r="R14" s="28" t="b">
+        <v>0</v>
+      </c>
+      <c r="S14" s="28" t="b">
+        <v>0</v>
+      </c>
+      <c r="T14" s="28" t="b">
+        <v>0</v>
+      </c>
+      <c r="U14" s="28" t="b">
+        <v>0</v>
+      </c>
+      <c r="V14" s="28" t="b">
+        <v>0</v>
+      </c>
+      <c r="W14" s="28" t="b">
+        <v>0</v>
+      </c>
+      <c r="X14" s="28" t="b">
+        <v>0</v>
+      </c>
+      <c r="Y14" s="28" t="b">
+        <v>0</v>
+      </c>
+      <c r="Z14" s="28" t="b">
+        <v>0</v>
+      </c>
+      <c r="AA14" s="28" t="b">
+        <v>0</v>
+      </c>
+      <c r="AB14" s="28" t="b">
+        <v>0</v>
+      </c>
+      <c r="AC14" s="28" t="b">
+        <v>0</v>
+      </c>
+      <c r="AD14" s="28" t="b">
+        <v>0</v>
+      </c>
+      <c r="AE14" s="28" t="b">
+        <v>0</v>
+      </c>
+      <c r="AF14" s="28" t="b">
+        <v>0</v>
+      </c>
+      <c r="AG14" s="28" t="b">
+        <v>0</v>
+      </c>
+      <c r="AH14" s="28" t="b">
+        <v>0</v>
+      </c>
+      <c r="AI14" s="28" t="b">
+        <v>0</v>
+      </c>
+      <c r="AJ14" s="28" t="b">
+        <v>0</v>
+      </c>
+      <c r="AK14" s="28" t="b">
+        <v>0</v>
+      </c>
+      <c r="AL14" s="28" t="b">
+        <v>0</v>
+      </c>
+      <c r="AM14" s="28" t="b">
+        <v>0</v>
+      </c>
+      <c r="AN14" s="28" t="b">
+        <v>0</v>
+      </c>
+      <c r="AO14" s="31" t="b">
+        <v>0</v>
+      </c>
+      <c r="AP14" s="31" t="b">
+        <v>0</v>
+      </c>
+      <c r="AQ14" s="31" t="b">
+        <v>0</v>
+      </c>
+      <c r="AR14" s="31"/>
     </row>
     <row r="23" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A23" s="1"/>
@@ -2441,6 +2592,9 @@
     </row>
     <row r="27" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A27" s="1"/>
+    </row>
+    <row r="28" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A28" s="1"/>
     </row>
   </sheetData>
   <mergeCells count="11">

</xml_diff>

<commit_message>
further work on lipidcane2g; update tests
</commit_message>
<xml_diff>
--- a/BioSTEAM 2.x.x/biorefineries/cornstover/_humbird2011.xlsx
+++ b/BioSTEAM 2.x.x/biorefineries/cornstover/_humbird2011.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23801"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23929"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/733a0933307f0df0/Code/Bioindustrial-Park/BioSTEAM 2.x.x/biorefineries/cornstover/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="76" documentId="11_93738BBF658B224CE52DD40E9AAED54DBB468F57" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{8FBAE52F-AB7D-4B05-99DD-98324BB7C5D0}"/>
+  <xr:revisionPtr revIDLastSave="80" documentId="11_93738BBF658B224CE52DD40E9AAED54DBB468F57" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{DD778C37-AC60-40BA-BE90-9BB9C76D6AD9}"/>
   <bookViews>
-    <workbookView minimized="1" xWindow="2508" yWindow="2820" windowWidth="20532" windowHeight="10980" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2508" yWindow="2652" windowWidth="20532" windowHeight="10980" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -155,9 +155,6 @@
     <t>Seed Hold Tank</t>
   </si>
   <si>
-    <t>HXutility-Hydrolysate Cooler</t>
-  </si>
-  <si>
     <t>Mixer-Enzyme Hydrolysate Mixer</t>
   </si>
   <si>
@@ -201,6 +198,9 @@
   </si>
   <si>
     <t>Lower bound</t>
+  </si>
+  <si>
+    <t>HXutility-Hydrolysate Heat Exchanger</t>
   </si>
 </sst>
 </file>
@@ -696,8 +696,8 @@
   <dimension ref="A1:AR28"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="62" zoomScaleNormal="62" workbookViewId="0">
-      <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="AN13" sqref="AN13"/>
+      <pane xSplit="1" topLeftCell="AC1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="T13" sqref="T13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -752,7 +752,7 @@
         <v>31</v>
       </c>
       <c r="H1" s="34" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="I1" s="34"/>
       <c r="J1" s="34"/>
@@ -762,11 +762,11 @@
       <c r="L1" s="34"/>
       <c r="M1" s="34"/>
       <c r="N1" s="34" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="O1" s="34"/>
       <c r="P1" s="5" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="Q1" s="34" t="s">
         <v>33</v>
@@ -776,7 +776,7 @@
         <v>34</v>
       </c>
       <c r="T1" s="6" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="U1" s="6" t="s">
         <v>35</v>
@@ -793,37 +793,37 @@
       <c r="Y1" s="35"/>
       <c r="Z1" s="35"/>
       <c r="AA1" s="15" t="s">
+        <v>54</v>
+      </c>
+      <c r="AB1" s="15" t="s">
         <v>39</v>
       </c>
-      <c r="AB1" s="15" t="s">
+      <c r="AC1" s="35" t="s">
         <v>40</v>
-      </c>
-      <c r="AC1" s="35" t="s">
-        <v>41</v>
       </c>
       <c r="AD1" s="35"/>
       <c r="AE1" s="35"/>
       <c r="AF1" s="34" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="AG1" s="34"/>
       <c r="AH1" s="34"/>
       <c r="AI1" s="34" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="AJ1" s="34"/>
       <c r="AK1" s="34"/>
       <c r="AL1" s="34"/>
       <c r="AM1" s="34" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="AN1" s="34"/>
       <c r="AO1" s="34" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="AP1" s="34"/>
       <c r="AQ1" s="26" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="AR1" s="26"/>
     </row>
@@ -940,7 +940,7 @@
         <v>15</v>
       </c>
       <c r="AL2" s="7" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="AM2" s="24" t="s">
         <v>8</v>
@@ -949,7 +949,7 @@
         <v>16</v>
       </c>
       <c r="AO2" s="7" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="AP2" s="7" t="s">
         <v>16</v>
@@ -1277,10 +1277,10 @@
         <v>410369</v>
       </c>
       <c r="S5" s="10">
-        <v>-8</v>
+        <v>8</v>
       </c>
       <c r="T5" s="11">
-        <v>-2</v>
+        <v>2</v>
       </c>
       <c r="U5" s="11">
         <v>402194</v>
@@ -1301,7 +1301,7 @@
         <v>40414</v>
       </c>
       <c r="AA5" s="11">
-        <v>-8</v>
+        <v>8</v>
       </c>
       <c r="AB5" s="11">
         <v>380000</v>
@@ -1355,7 +1355,7 @@
     </row>
     <row r="6" spans="1:44" s="32" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A6" s="12" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B6" s="32" t="b">
         <f>FALSE</f>
@@ -2448,7 +2448,7 @@
     </row>
     <row r="14" spans="1:44" x14ac:dyDescent="0.3">
       <c r="A14" s="29" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B14" s="28" t="b">
         <v>0</v>

</xml_diff>